<commit_message>
Refactor (dependo) + content update
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35945CC7-96F7-B04C-99B7-73D39A435A29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D408629-BD27-4441-926B-9217AF18E231}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6880" yWindow="2520" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1717" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="277">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -858,6 +858,12 @@
   </si>
   <si>
     <t>dependo.87-megaderma</t>
+  </si>
+  <si>
+    <t>ADAMTS2</t>
+  </si>
+  <si>
+    <t>dependo.88-Megaderma</t>
   </si>
 </sst>
 </file>
@@ -3347,13 +3353,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26DACFF6-840F-D741-97EA-4F87EFFABC86}">
-  <dimension ref="A1:FH86"/>
+  <dimension ref="A1:FH87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X41" sqref="A1:AA73"/>
+      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13789,8 +13795,8 @@
       <c r="E51" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="F51" s="23" t="s">
-        <v>172</v>
+      <c r="F51" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="G51" s="25">
         <v>1</v>
@@ -13813,11 +13819,11 @@
       <c r="M51" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N51" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O51" s="14" t="s">
-        <v>22</v>
+      <c r="N51" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P51" s="3" t="s">
         <v>84</v>
@@ -13995,61 +14001,57 @@
     </row>
     <row r="52" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>232</v>
+        <v>276</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C52" s="25">
-        <v>86</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>21</v>
+        <v>88</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>15</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>172</v>
+        <v>240</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>118</v>
       </c>
       <c r="G52" s="25">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H52" s="25">
-        <v>5</v>
-      </c>
-      <c r="I52" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="N52" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="O52" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I52" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="Q52" s="33" t="s">
-        <v>118</v>
-      </c>
+      <c r="J52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="33"/>
       <c r="R52" s="10" t="s">
-        <v>197</v>
+        <v>275</v>
       </c>
       <c r="S52" s="10" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
       <c r="T52" s="8" t="s">
         <v>43</v>
@@ -14061,10 +14063,10 @@
         <v>216</v>
       </c>
       <c r="W52" s="20" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="X52" s="20" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="Y52" s="20" t="s">
         <v>2</v>
@@ -14215,59 +14217,61 @@
     </row>
     <row r="53" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>213</v>
+        <v>232</v>
       </c>
       <c r="B53" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C53" s="25">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="G53" s="27">
-        <v>1</v>
-      </c>
-      <c r="H53" s="27">
-        <v>1</v>
-      </c>
-      <c r="I53" s="27"/>
-      <c r="J53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N53" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>43</v>
+        <v>120</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G53" s="25">
+        <v>5</v>
+      </c>
+      <c r="H53" s="25">
+        <v>5</v>
+      </c>
+      <c r="I53" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="P53" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Q53" s="34" t="s">
-        <v>191</v>
+      <c r="Q53" s="33" t="s">
+        <v>118</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="S53" s="10" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
       <c r="T53" s="8" t="s">
         <v>43</v>
@@ -14279,10 +14283,10 @@
         <v>216</v>
       </c>
       <c r="W53" s="20" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="X53" s="20" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="Y53" s="20" t="s">
         <v>2</v>
@@ -14433,73 +14437,74 @@
     </row>
     <row r="54" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B54" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C54" s="25">
-        <v>160</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>40</v>
+        <v>92</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>159</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="G54" s="25">
+        <v>192</v>
+      </c>
+      <c r="G54" s="27">
         <v>1</v>
       </c>
-      <c r="H54" s="25">
+      <c r="H54" s="27">
         <v>1</v>
       </c>
-      <c r="I54" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="J54" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="K54" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N54" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="O54" s="3" t="s">
-        <v>42</v>
+      <c r="I54" s="27"/>
+      <c r="J54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P54" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Q54" s="10" t="s">
+      <c r="Q54" s="34" t="s">
         <v>191</v>
       </c>
       <c r="R54" s="10" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="S54" s="10" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="T54" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U54" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V54" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W54" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="X54" s="20" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="Y54" s="20" t="s">
         <v>2</v>
@@ -14650,76 +14655,73 @@
     </row>
     <row r="55" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="B55" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C55" s="25">
-        <v>174</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="F55" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F55" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="G55" s="27">
+      <c r="G55" s="25">
         <v>1</v>
       </c>
-      <c r="H55" s="27">
+      <c r="H55" s="25">
         <v>1</v>
       </c>
       <c r="I55" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="J55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="N55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O55" s="4" t="s">
-        <v>43</v>
+      <c r="J55" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="P55" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Q55" s="33" t="s">
-        <v>118</v>
+      <c r="Q55" s="10" t="s">
+        <v>191</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="T55" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U55" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V55" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W55" s="20" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="X55" s="20" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="Y55" s="20" t="s">
         <v>2</v>
@@ -14868,30 +14870,30 @@
       <c r="FG55" s="24"/>
       <c r="FH55" s="24"/>
     </row>
-    <row r="56" spans="1:164" s="26" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>224</v>
+        <v>166</v>
       </c>
       <c r="B56" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C56" s="25">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D56" s="27" t="s">
         <v>15</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="F56" s="23" t="s">
         <v>172</v>
       </c>
       <c r="G56" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H56" s="27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56" s="27" t="s">
         <v>191</v>
@@ -14921,10 +14923,10 @@
         <v>118</v>
       </c>
       <c r="R56" s="10" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="S56" s="10" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="T56" s="8" t="s">
         <v>43</v>
@@ -14936,10 +14938,10 @@
         <v>216</v>
       </c>
       <c r="W56" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="X56" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Y56" s="20" t="s">
         <v>2</v>
@@ -15090,49 +15092,49 @@
     </row>
     <row r="57" spans="1:164" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="B57" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C57" s="25">
-        <v>187</v>
-      </c>
-      <c r="D57" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="D57" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E57" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="F57" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="G57" s="25">
-        <v>1</v>
-      </c>
-      <c r="H57" s="25">
-        <v>1</v>
-      </c>
-      <c r="I57" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="J57" s="13" t="s">
-        <v>130</v>
+      <c r="E57" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="F57" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="G57" s="27">
+        <v>2</v>
+      </c>
+      <c r="H57" s="27">
+        <v>2</v>
+      </c>
+      <c r="I57" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L57" s="13" t="s">
-        <v>130</v>
+      <c r="L57" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N57" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="14" t="s">
-        <v>22</v>
+      <c r="N57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P57" s="3" t="s">
         <v>84</v>
@@ -15141,10 +15143,10 @@
         <v>118</v>
       </c>
       <c r="R57" s="10" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
       <c r="S57" s="10" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="T57" s="8" t="s">
         <v>43</v>
@@ -15156,10 +15158,10 @@
         <v>216</v>
       </c>
       <c r="W57" s="20" t="s">
-        <v>252</v>
+        <v>168</v>
       </c>
       <c r="X57" s="20" t="s">
-        <v>252</v>
+        <v>168</v>
       </c>
       <c r="Y57" s="20" t="s">
         <v>2</v>
@@ -15308,23 +15310,23 @@
       <c r="FG57" s="24"/>
       <c r="FH57" s="24"/>
     </row>
-    <row r="58" spans="1:164" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:164" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B58" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C58" s="25">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D58" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="F58" s="20" t="s">
         <v>192</v>
       </c>
       <c r="G58" s="25">
@@ -15333,24 +15335,26 @@
       <c r="H58" s="25">
         <v>1</v>
       </c>
-      <c r="I58" s="25"/>
-      <c r="J58" s="4" t="s">
-        <v>43</v>
+      <c r="I58" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="J58" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L58" s="4" t="s">
-        <v>43</v>
+      <c r="L58" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N58" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O58" s="4" t="s">
-        <v>43</v>
+      <c r="N58" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O58" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="P58" s="3" t="s">
         <v>84</v>
@@ -15359,23 +15363,25 @@
         <v>118</v>
       </c>
       <c r="R58" s="10" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="S58" s="10" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="T58" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U58" s="7"/>
+      <c r="U58" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="V58" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W58" s="20" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="X58" s="20" t="s">
-        <v>214</v>
+        <v>252</v>
       </c>
       <c r="Y58" s="20" t="s">
         <v>2</v>
@@ -15524,15 +15530,15 @@
       <c r="FG58" s="24"/>
       <c r="FH58" s="24"/>
     </row>
-    <row r="59" spans="1:164" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>214</v>
+        <v>243</v>
       </c>
       <c r="B59" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C59" s="25">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D59" s="25" t="s">
         <v>14</v>
@@ -15543,11 +15549,11 @@
       <c r="F59" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="G59" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H59" s="25" t="s">
-        <v>118</v>
+      <c r="G59" s="25">
+        <v>1</v>
+      </c>
+      <c r="H59" s="25">
+        <v>1</v>
       </c>
       <c r="I59" s="25"/>
       <c r="J59" s="4" t="s">
@@ -15575,10 +15581,10 @@
         <v>118</v>
       </c>
       <c r="R59" s="10" t="s">
-        <v>72</v>
+        <v>244</v>
       </c>
       <c r="S59" s="10" t="s">
-        <v>73</v>
+        <v>245</v>
       </c>
       <c r="T59" s="8" t="s">
         <v>43</v>
@@ -15742,13 +15748,13 @@
     </row>
     <row r="60" spans="1:164" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B60" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C60" s="25">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D60" s="25" t="s">
         <v>14</v>
@@ -15791,22 +15797,23 @@
         <v>118</v>
       </c>
       <c r="R60" s="10" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="S60" s="10" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="T60" s="8" t="s">
         <v>43</v>
       </c>
+      <c r="U60" s="7"/>
       <c r="V60" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W60" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X60" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y60" s="20" t="s">
         <v>2</v>
@@ -15955,51 +15962,49 @@
       <c r="FG60" s="24"/>
       <c r="FH60" s="24"/>
     </row>
-    <row r="61" spans="1:164" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:164" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="C61" s="25">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D61" s="25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E61" s="22" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="F61" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="G61" s="29">
-        <v>1</v>
-      </c>
-      <c r="H61" s="29">
-        <v>1</v>
-      </c>
-      <c r="I61" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="J61" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K61" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L61" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N61" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O61" s="14" t="s">
-        <v>22</v>
+      <c r="G61" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="H61" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I61" s="25"/>
+      <c r="J61" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M61" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N61" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P61" s="3" t="s">
         <v>84</v>
@@ -16007,24 +16012,23 @@
       <c r="Q61" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R61" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S61" s="11" t="s">
-        <v>43</v>
+      <c r="R61" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S61" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="T61" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U61" s="7"/>
       <c r="V61" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W61" s="20" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="X61" s="20" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="Y61" s="20" t="s">
         <v>2</v>
@@ -16175,13 +16179,13 @@
     </row>
     <row r="62" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="25" t="s">
         <v>84</v>
       </c>
       <c r="C62" s="25">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D62" s="25" t="s">
         <v>15</v>
@@ -16201,17 +16205,17 @@
       <c r="I62" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="J62" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>133</v>
+      <c r="J62" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M62" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="N62" s="14" t="s">
         <v>22</v>
@@ -16234,14 +16238,15 @@
       <c r="T62" s="8" t="s">
         <v>43</v>
       </c>
+      <c r="U62" s="7"/>
       <c r="V62" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W62" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X62" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y62" s="20" t="s">
         <v>2</v>
@@ -16392,13 +16397,13 @@
     </row>
     <row r="63" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B63" s="25" t="s">
         <v>84</v>
       </c>
       <c r="C63" s="25">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D63" s="25" t="s">
         <v>15</v>
@@ -16418,17 +16423,17 @@
       <c r="I63" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="J63" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="M63" s="2" t="s">
-        <v>85</v>
+      <c r="J63" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="N63" s="14" t="s">
         <v>22</v>
@@ -16442,24 +16447,23 @@
       <c r="Q63" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R63" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="S63" s="10" t="s">
-        <v>54</v>
+      <c r="R63" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S63" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="T63" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U63" s="7"/>
       <c r="V63" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W63" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X63" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y63" s="20" t="s">
         <v>2</v>
@@ -16610,43 +16614,43 @@
     </row>
     <row r="64" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>191</v>
+        <v>84</v>
       </c>
       <c r="C64" s="25">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D64" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="E64" s="23" t="s">
-        <v>147</v>
+      <c r="E64" s="22" t="s">
+        <v>94</v>
       </c>
       <c r="F64" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="G64" s="27">
+      <c r="G64" s="29">
         <v>1</v>
       </c>
-      <c r="H64" s="27">
+      <c r="H64" s="29">
         <v>1</v>
       </c>
       <c r="I64" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="J64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="L64" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M64" s="4" t="s">
-        <v>43</v>
+      <c r="J64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K64" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M64" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="N64" s="14" t="s">
         <v>22</v>
@@ -16660,26 +16664,24 @@
       <c r="Q64" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R64" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S64" s="11" t="s">
-        <v>43</v>
+      <c r="R64" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="S64" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="T64" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U64" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="U64" s="7"/>
       <c r="V64" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W64" s="20" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="X64" s="20" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="Y64" s="20" t="s">
         <v>2</v>
@@ -16830,22 +16832,22 @@
     </row>
     <row r="65" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="B65" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C65" s="25">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D65" s="25" t="s">
         <v>15</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>193</v>
+        <v>147</v>
+      </c>
+      <c r="F65" s="22" t="s">
+        <v>192</v>
       </c>
       <c r="G65" s="27">
         <v>1</v>
@@ -16853,8 +16855,8 @@
       <c r="H65" s="27">
         <v>1</v>
       </c>
-      <c r="I65" s="25" t="s">
-        <v>191</v>
+      <c r="I65" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>43</v>
@@ -16868,11 +16870,11 @@
       <c r="M65" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N65" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O65" s="4" t="s">
-        <v>43</v>
+      <c r="N65" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O65" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="P65" s="3" t="s">
         <v>84</v>
@@ -16880,11 +16882,11 @@
       <c r="Q65" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R65" s="10" t="s">
-        <v>180</v>
-      </c>
-      <c r="S65" s="10" t="s">
-        <v>181</v>
+      <c r="R65" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S65" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="T65" s="8" t="s">
         <v>43</v>
@@ -16896,10 +16898,10 @@
         <v>216</v>
       </c>
       <c r="W65" s="20" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="X65" s="20" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
       <c r="Y65" s="20" t="s">
         <v>2</v>
@@ -17050,22 +17052,22 @@
     </row>
     <row r="66" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="C66" s="25">
-        <v>221</v>
-      </c>
-      <c r="D66" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D66" s="25" t="s">
         <v>15</v>
       </c>
       <c r="E66" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F66" s="22" t="s">
-        <v>192</v>
+        <v>146</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="G66" s="27">
         <v>1</v>
@@ -17083,16 +17085,16 @@
         <v>43</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="M66" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="N66" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O66" s="14" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="M66" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N66" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>84</v>
@@ -17101,10 +17103,10 @@
         <v>118</v>
       </c>
       <c r="R66" s="10" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="S66" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="T66" s="8" t="s">
         <v>43</v>
@@ -17116,10 +17118,10 @@
         <v>216</v>
       </c>
       <c r="W66" s="20" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="X66" s="20" t="s">
-        <v>152</v>
+        <v>182</v>
       </c>
       <c r="Y66" s="20" t="s">
         <v>2</v>
@@ -17270,28 +17272,28 @@
     </row>
     <row r="67" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>191</v>
+        <v>84</v>
       </c>
       <c r="C67" s="25">
-        <v>365</v>
-      </c>
-      <c r="D67" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E67" s="22" t="s">
-        <v>95</v>
+        <v>221</v>
+      </c>
+      <c r="D67" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="23" t="s">
+        <v>153</v>
       </c>
       <c r="F67" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="G67" s="25">
-        <v>7</v>
-      </c>
-      <c r="H67" s="25">
-        <v>7</v>
+      <c r="G67" s="27">
+        <v>1</v>
+      </c>
+      <c r="H67" s="27">
+        <v>1</v>
       </c>
       <c r="I67" s="25" t="s">
         <v>191</v>
@@ -17303,10 +17305,10 @@
         <v>43</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="M67" s="4" t="s">
-        <v>43</v>
+        <v>132</v>
+      </c>
+      <c r="M67" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="N67" s="14" t="s">
         <v>22</v>
@@ -17321,10 +17323,10 @@
         <v>118</v>
       </c>
       <c r="R67" s="10" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="S67" s="10" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="T67" s="8" t="s">
         <v>43</v>
@@ -17336,10 +17338,10 @@
         <v>216</v>
       </c>
       <c r="W67" s="20" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="X67" s="20" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="Y67" s="20" t="s">
         <v>2</v>
@@ -17350,16 +17352,153 @@
       <c r="AA67" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="AB67" s="24"/>
+      <c r="AC67" s="24"/>
+      <c r="AD67" s="24"/>
+      <c r="AE67" s="24"/>
+      <c r="AF67" s="24"/>
+      <c r="AG67" s="24"/>
+      <c r="AH67" s="24"/>
+      <c r="AI67" s="24"/>
+      <c r="AJ67" s="24"/>
+      <c r="AK67" s="24"/>
+      <c r="AL67" s="24"/>
+      <c r="AM67" s="24"/>
+      <c r="AN67" s="24"/>
+      <c r="AO67" s="24"/>
+      <c r="AP67" s="24"/>
+      <c r="AQ67" s="24"/>
+      <c r="AR67" s="24"/>
+      <c r="AS67" s="24"/>
+      <c r="AT67" s="24"/>
+      <c r="AU67" s="24"/>
+      <c r="AV67" s="24"/>
+      <c r="AW67" s="24"/>
+      <c r="AX67" s="24"/>
+      <c r="AY67" s="24"/>
+      <c r="AZ67" s="24"/>
+      <c r="BA67" s="24"/>
+      <c r="BB67" s="24"/>
+      <c r="BC67" s="24"/>
+      <c r="BD67" s="24"/>
+      <c r="BE67" s="24"/>
+      <c r="BF67" s="24"/>
+      <c r="BG67" s="24"/>
+      <c r="BH67" s="24"/>
+      <c r="BI67" s="24"/>
+      <c r="BJ67" s="24"/>
+      <c r="BK67" s="24"/>
+      <c r="BL67" s="24"/>
+      <c r="BM67" s="24"/>
+      <c r="BN67" s="24"/>
+      <c r="BO67" s="24"/>
+      <c r="BP67" s="24"/>
+      <c r="BQ67" s="24"/>
+      <c r="BR67" s="24"/>
+      <c r="BS67" s="24"/>
+      <c r="BT67" s="24"/>
+      <c r="BU67" s="24"/>
+      <c r="BV67" s="24"/>
+      <c r="BW67" s="24"/>
+      <c r="BX67" s="24"/>
+      <c r="BY67" s="24"/>
+      <c r="BZ67" s="24"/>
+      <c r="CA67" s="24"/>
+      <c r="CB67" s="24"/>
+      <c r="CC67" s="24"/>
+      <c r="CD67" s="24"/>
+      <c r="CE67" s="24"/>
+      <c r="CF67" s="24"/>
+      <c r="CG67" s="24"/>
+      <c r="CH67" s="24"/>
+      <c r="CI67" s="24"/>
+      <c r="CJ67" s="24"/>
+      <c r="CK67" s="24"/>
+      <c r="CL67" s="24"/>
+      <c r="CM67" s="24"/>
+      <c r="CN67" s="24"/>
+      <c r="CO67" s="24"/>
+      <c r="CP67" s="24"/>
+      <c r="CQ67" s="24"/>
+      <c r="CR67" s="24"/>
+      <c r="CS67" s="24"/>
+      <c r="CT67" s="24"/>
+      <c r="CU67" s="24"/>
+      <c r="CV67" s="24"/>
+      <c r="CW67" s="24"/>
+      <c r="CX67" s="24"/>
+      <c r="CY67" s="24"/>
+      <c r="CZ67" s="24"/>
+      <c r="DA67" s="24"/>
+      <c r="DB67" s="24"/>
+      <c r="DC67" s="24"/>
+      <c r="DD67" s="24"/>
+      <c r="DE67" s="24"/>
+      <c r="DF67" s="24"/>
+      <c r="DG67" s="24"/>
+      <c r="DH67" s="24"/>
+      <c r="DI67" s="24"/>
+      <c r="DJ67" s="24"/>
+      <c r="DK67" s="24"/>
+      <c r="DL67" s="24"/>
+      <c r="DM67" s="24"/>
+      <c r="DN67" s="24"/>
+      <c r="DO67" s="24"/>
+      <c r="DP67" s="24"/>
+      <c r="DQ67" s="24"/>
+      <c r="DR67" s="24"/>
+      <c r="DS67" s="24"/>
+      <c r="DT67" s="24"/>
+      <c r="DU67" s="24"/>
+      <c r="DV67" s="24"/>
+      <c r="DW67" s="24"/>
+      <c r="DX67" s="24"/>
+      <c r="DY67" s="24"/>
+      <c r="DZ67" s="24"/>
+      <c r="EA67" s="24"/>
+      <c r="EB67" s="24"/>
+      <c r="EC67" s="24"/>
+      <c r="ED67" s="24"/>
+      <c r="EE67" s="24"/>
+      <c r="EF67" s="24"/>
+      <c r="EG67" s="24"/>
+      <c r="EH67" s="24"/>
+      <c r="EI67" s="24"/>
+      <c r="EJ67" s="24"/>
+      <c r="EK67" s="24"/>
+      <c r="EL67" s="24"/>
+      <c r="EM67" s="24"/>
+      <c r="EN67" s="24"/>
+      <c r="EO67" s="24"/>
+      <c r="EP67" s="24"/>
+      <c r="EQ67" s="24"/>
+      <c r="ER67" s="24"/>
+      <c r="ES67" s="24"/>
+      <c r="ET67" s="24"/>
+      <c r="EU67" s="24"/>
+      <c r="EV67" s="24"/>
+      <c r="EW67" s="24"/>
+      <c r="EX67" s="24"/>
+      <c r="EY67" s="24"/>
+      <c r="EZ67" s="24"/>
+      <c r="FA67" s="24"/>
+      <c r="FB67" s="24"/>
+      <c r="FC67" s="24"/>
+      <c r="FD67" s="24"/>
+      <c r="FE67" s="24"/>
+      <c r="FF67" s="24"/>
+      <c r="FG67" s="24"/>
+      <c r="FH67" s="24"/>
     </row>
     <row r="68" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B68" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C68" s="25">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>14</v>
@@ -17371,10 +17510,10 @@
         <v>192</v>
       </c>
       <c r="G68" s="25">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="H68" s="25">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="I68" s="25" t="s">
         <v>191</v>
@@ -17404,10 +17543,10 @@
         <v>118</v>
       </c>
       <c r="R68" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="S68" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T68" s="8" t="s">
         <v>43</v>
@@ -17419,10 +17558,10 @@
         <v>216</v>
       </c>
       <c r="W68" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X68" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Y68" s="20" t="s">
         <v>2</v>
@@ -17433,177 +17572,40 @@
       <c r="AA68" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AB68" s="24"/>
-      <c r="AC68" s="24"/>
-      <c r="AD68" s="24"/>
-      <c r="AE68" s="24"/>
-      <c r="AF68" s="24"/>
-      <c r="AG68" s="24"/>
-      <c r="AH68" s="24"/>
-      <c r="AI68" s="24"/>
-      <c r="AJ68" s="24"/>
-      <c r="AK68" s="24"/>
-      <c r="AL68" s="24"/>
-      <c r="AM68" s="24"/>
-      <c r="AN68" s="24"/>
-      <c r="AO68" s="24"/>
-      <c r="AP68" s="24"/>
-      <c r="AQ68" s="24"/>
-      <c r="AR68" s="24"/>
-      <c r="AS68" s="24"/>
-      <c r="AT68" s="24"/>
-      <c r="AU68" s="24"/>
-      <c r="AV68" s="24"/>
-      <c r="AW68" s="24"/>
-      <c r="AX68" s="24"/>
-      <c r="AY68" s="24"/>
-      <c r="AZ68" s="24"/>
-      <c r="BA68" s="24"/>
-      <c r="BB68" s="24"/>
-      <c r="BC68" s="24"/>
-      <c r="BD68" s="24"/>
-      <c r="BE68" s="24"/>
-      <c r="BF68" s="24"/>
-      <c r="BG68" s="24"/>
-      <c r="BH68" s="24"/>
-      <c r="BI68" s="24"/>
-      <c r="BJ68" s="24"/>
-      <c r="BK68" s="24"/>
-      <c r="BL68" s="24"/>
-      <c r="BM68" s="24"/>
-      <c r="BN68" s="24"/>
-      <c r="BO68" s="24"/>
-      <c r="BP68" s="24"/>
-      <c r="BQ68" s="24"/>
-      <c r="BR68" s="24"/>
-      <c r="BS68" s="24"/>
-      <c r="BT68" s="24"/>
-      <c r="BU68" s="24"/>
-      <c r="BV68" s="24"/>
-      <c r="BW68" s="24"/>
-      <c r="BX68" s="24"/>
-      <c r="BY68" s="24"/>
-      <c r="BZ68" s="24"/>
-      <c r="CA68" s="24"/>
-      <c r="CB68" s="24"/>
-      <c r="CC68" s="24"/>
-      <c r="CD68" s="24"/>
-      <c r="CE68" s="24"/>
-      <c r="CF68" s="24"/>
-      <c r="CG68" s="24"/>
-      <c r="CH68" s="24"/>
-      <c r="CI68" s="24"/>
-      <c r="CJ68" s="24"/>
-      <c r="CK68" s="24"/>
-      <c r="CL68" s="24"/>
-      <c r="CM68" s="24"/>
-      <c r="CN68" s="24"/>
-      <c r="CO68" s="24"/>
-      <c r="CP68" s="24"/>
-      <c r="CQ68" s="24"/>
-      <c r="CR68" s="24"/>
-      <c r="CS68" s="24"/>
-      <c r="CT68" s="24"/>
-      <c r="CU68" s="24"/>
-      <c r="CV68" s="24"/>
-      <c r="CW68" s="24"/>
-      <c r="CX68" s="24"/>
-      <c r="CY68" s="24"/>
-      <c r="CZ68" s="24"/>
-      <c r="DA68" s="24"/>
-      <c r="DB68" s="24"/>
-      <c r="DC68" s="24"/>
-      <c r="DD68" s="24"/>
-      <c r="DE68" s="24"/>
-      <c r="DF68" s="24"/>
-      <c r="DG68" s="24"/>
-      <c r="DH68" s="24"/>
-      <c r="DI68" s="24"/>
-      <c r="DJ68" s="24"/>
-      <c r="DK68" s="24"/>
-      <c r="DL68" s="24"/>
-      <c r="DM68" s="24"/>
-      <c r="DN68" s="24"/>
-      <c r="DO68" s="24"/>
-      <c r="DP68" s="24"/>
-      <c r="DQ68" s="24"/>
-      <c r="DR68" s="24"/>
-      <c r="DS68" s="24"/>
-      <c r="DT68" s="24"/>
-      <c r="DU68" s="24"/>
-      <c r="DV68" s="24"/>
-      <c r="DW68" s="24"/>
-      <c r="DX68" s="24"/>
-      <c r="DY68" s="24"/>
-      <c r="DZ68" s="24"/>
-      <c r="EA68" s="24"/>
-      <c r="EB68" s="24"/>
-      <c r="EC68" s="24"/>
-      <c r="ED68" s="24"/>
-      <c r="EE68" s="24"/>
-      <c r="EF68" s="24"/>
-      <c r="EG68" s="24"/>
-      <c r="EH68" s="24"/>
-      <c r="EI68" s="24"/>
-      <c r="EJ68" s="24"/>
-      <c r="EK68" s="24"/>
-      <c r="EL68" s="24"/>
-      <c r="EM68" s="24"/>
-      <c r="EN68" s="24"/>
-      <c r="EO68" s="24"/>
-      <c r="EP68" s="24"/>
-      <c r="EQ68" s="24"/>
-      <c r="ER68" s="24"/>
-      <c r="ES68" s="24"/>
-      <c r="ET68" s="24"/>
-      <c r="EU68" s="24"/>
-      <c r="EV68" s="24"/>
-      <c r="EW68" s="24"/>
-      <c r="EX68" s="24"/>
-      <c r="EY68" s="24"/>
-      <c r="EZ68" s="24"/>
-      <c r="FA68" s="24"/>
-      <c r="FB68" s="24"/>
-      <c r="FC68" s="24"/>
-      <c r="FD68" s="24"/>
-      <c r="FE68" s="24"/>
-      <c r="FF68" s="24"/>
-      <c r="FG68" s="24"/>
-      <c r="FH68" s="24"/>
     </row>
     <row r="69" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C69" s="25">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E69" s="23" t="s">
-        <v>145</v>
+        <v>14</v>
+      </c>
+      <c r="E69" s="22" t="s">
+        <v>95</v>
       </c>
       <c r="F69" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="G69" s="27">
-        <v>1</v>
-      </c>
-      <c r="H69" s="27">
-        <v>1</v>
+      <c r="G69" s="25">
+        <v>20</v>
+      </c>
+      <c r="H69" s="25">
+        <v>20</v>
       </c>
       <c r="I69" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="J69" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="K69" s="21" t="s">
-        <v>139</v>
+      <c r="J69" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="L69" s="4" t="s">
         <v>43</v>
@@ -17623,24 +17625,26 @@
       <c r="Q69" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R69" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S69" s="11" t="s">
-        <v>43</v>
+      <c r="R69" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="S69" s="10" t="s">
+        <v>150</v>
       </c>
       <c r="T69" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U69" s="7"/>
+      <c r="U69" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="V69" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W69" s="20" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="X69" s="20" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="Y69" s="20" t="s">
         <v>2</v>
@@ -17791,37 +17795,37 @@
     </row>
     <row r="70" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="B70" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C70" s="25">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D70" s="25" t="s">
         <v>15</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>258</v>
+        <v>145</v>
       </c>
       <c r="F70" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="G70" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H70" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="I70" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K70" s="4" t="s">
-        <v>43</v>
+        <v>192</v>
+      </c>
+      <c r="G70" s="27">
+        <v>1</v>
+      </c>
+      <c r="H70" s="27">
+        <v>1</v>
+      </c>
+      <c r="I70" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="J70" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K70" s="21" t="s">
+        <v>139</v>
       </c>
       <c r="L70" s="4" t="s">
         <v>43</v>
@@ -17829,11 +17833,11 @@
       <c r="M70" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N70" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="O70" s="4" t="s">
-        <v>43</v>
+      <c r="N70" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O70" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="P70" s="3" t="s">
         <v>84</v>
@@ -17841,11 +17845,11 @@
       <c r="Q70" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R70" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="S70" s="10" t="s">
-        <v>260</v>
+      <c r="R70" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S70" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="T70" s="8" t="s">
         <v>43</v>
@@ -17855,10 +17859,10 @@
         <v>216</v>
       </c>
       <c r="W70" s="20" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="X70" s="20" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="Y70" s="20" t="s">
         <v>2</v>
@@ -18009,49 +18013,49 @@
     </row>
     <row r="71" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="B71" s="25" t="s">
         <v>191</v>
       </c>
       <c r="C71" s="25">
-        <v>500</v>
+        <v>372</v>
       </c>
       <c r="D71" s="25" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>136</v>
+        <v>258</v>
       </c>
       <c r="F71" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="G71" s="27">
-        <v>1</v>
-      </c>
-      <c r="H71" s="27">
-        <v>1</v>
-      </c>
-      <c r="I71" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="J71" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="K71" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="L71" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="M71" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="N71" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="O71" s="14" t="s">
-        <v>22</v>
+        <v>118</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I71" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M71" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O71" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="P71" s="3" t="s">
         <v>84</v>
@@ -18059,40 +18063,175 @@
       <c r="Q71" s="33" t="s">
         <v>118</v>
       </c>
-      <c r="R71" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S71" s="11" t="s">
-        <v>43</v>
+      <c r="R71" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="S71" s="10" t="s">
+        <v>260</v>
       </c>
       <c r="T71" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U71" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="U71" s="7"/>
       <c r="V71" s="8" t="s">
         <v>216</v>
       </c>
       <c r="W71" s="20" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="X71" s="20" t="s">
-        <v>134</v>
+        <v>257</v>
       </c>
       <c r="Y71" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z71" s="20" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="AA71" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="AB71" s="24"/>
+      <c r="AC71" s="24"/>
+      <c r="AD71" s="24"/>
+      <c r="AE71" s="24"/>
+      <c r="AF71" s="24"/>
+      <c r="AG71" s="24"/>
+      <c r="AH71" s="24"/>
+      <c r="AI71" s="24"/>
+      <c r="AJ71" s="24"/>
+      <c r="AK71" s="24"/>
+      <c r="AL71" s="24"/>
+      <c r="AM71" s="24"/>
+      <c r="AN71" s="24"/>
+      <c r="AO71" s="24"/>
+      <c r="AP71" s="24"/>
+      <c r="AQ71" s="24"/>
+      <c r="AR71" s="24"/>
+      <c r="AS71" s="24"/>
+      <c r="AT71" s="24"/>
+      <c r="AU71" s="24"/>
+      <c r="AV71" s="24"/>
+      <c r="AW71" s="24"/>
+      <c r="AX71" s="24"/>
+      <c r="AY71" s="24"/>
+      <c r="AZ71" s="24"/>
+      <c r="BA71" s="24"/>
+      <c r="BB71" s="24"/>
+      <c r="BC71" s="24"/>
+      <c r="BD71" s="24"/>
+      <c r="BE71" s="24"/>
+      <c r="BF71" s="24"/>
+      <c r="BG71" s="24"/>
+      <c r="BH71" s="24"/>
+      <c r="BI71" s="24"/>
+      <c r="BJ71" s="24"/>
+      <c r="BK71" s="24"/>
+      <c r="BL71" s="24"/>
+      <c r="BM71" s="24"/>
+      <c r="BN71" s="24"/>
+      <c r="BO71" s="24"/>
+      <c r="BP71" s="24"/>
+      <c r="BQ71" s="24"/>
+      <c r="BR71" s="24"/>
+      <c r="BS71" s="24"/>
+      <c r="BT71" s="24"/>
+      <c r="BU71" s="24"/>
+      <c r="BV71" s="24"/>
+      <c r="BW71" s="24"/>
+      <c r="BX71" s="24"/>
+      <c r="BY71" s="24"/>
+      <c r="BZ71" s="24"/>
+      <c r="CA71" s="24"/>
+      <c r="CB71" s="24"/>
+      <c r="CC71" s="24"/>
+      <c r="CD71" s="24"/>
+      <c r="CE71" s="24"/>
+      <c r="CF71" s="24"/>
+      <c r="CG71" s="24"/>
+      <c r="CH71" s="24"/>
+      <c r="CI71" s="24"/>
+      <c r="CJ71" s="24"/>
+      <c r="CK71" s="24"/>
+      <c r="CL71" s="24"/>
+      <c r="CM71" s="24"/>
+      <c r="CN71" s="24"/>
+      <c r="CO71" s="24"/>
+      <c r="CP71" s="24"/>
+      <c r="CQ71" s="24"/>
+      <c r="CR71" s="24"/>
+      <c r="CS71" s="24"/>
+      <c r="CT71" s="24"/>
+      <c r="CU71" s="24"/>
+      <c r="CV71" s="24"/>
+      <c r="CW71" s="24"/>
+      <c r="CX71" s="24"/>
+      <c r="CY71" s="24"/>
+      <c r="CZ71" s="24"/>
+      <c r="DA71" s="24"/>
+      <c r="DB71" s="24"/>
+      <c r="DC71" s="24"/>
+      <c r="DD71" s="24"/>
+      <c r="DE71" s="24"/>
+      <c r="DF71" s="24"/>
+      <c r="DG71" s="24"/>
+      <c r="DH71" s="24"/>
+      <c r="DI71" s="24"/>
+      <c r="DJ71" s="24"/>
+      <c r="DK71" s="24"/>
+      <c r="DL71" s="24"/>
+      <c r="DM71" s="24"/>
+      <c r="DN71" s="24"/>
+      <c r="DO71" s="24"/>
+      <c r="DP71" s="24"/>
+      <c r="DQ71" s="24"/>
+      <c r="DR71" s="24"/>
+      <c r="DS71" s="24"/>
+      <c r="DT71" s="24"/>
+      <c r="DU71" s="24"/>
+      <c r="DV71" s="24"/>
+      <c r="DW71" s="24"/>
+      <c r="DX71" s="24"/>
+      <c r="DY71" s="24"/>
+      <c r="DZ71" s="24"/>
+      <c r="EA71" s="24"/>
+      <c r="EB71" s="24"/>
+      <c r="EC71" s="24"/>
+      <c r="ED71" s="24"/>
+      <c r="EE71" s="24"/>
+      <c r="EF71" s="24"/>
+      <c r="EG71" s="24"/>
+      <c r="EH71" s="24"/>
+      <c r="EI71" s="24"/>
+      <c r="EJ71" s="24"/>
+      <c r="EK71" s="24"/>
+      <c r="EL71" s="24"/>
+      <c r="EM71" s="24"/>
+      <c r="EN71" s="24"/>
+      <c r="EO71" s="24"/>
+      <c r="EP71" s="24"/>
+      <c r="EQ71" s="24"/>
+      <c r="ER71" s="24"/>
+      <c r="ES71" s="24"/>
+      <c r="ET71" s="24"/>
+      <c r="EU71" s="24"/>
+      <c r="EV71" s="24"/>
+      <c r="EW71" s="24"/>
+      <c r="EX71" s="24"/>
+      <c r="EY71" s="24"/>
+      <c r="EZ71" s="24"/>
+      <c r="FA71" s="24"/>
+      <c r="FB71" s="24"/>
+      <c r="FC71" s="24"/>
+      <c r="FD71" s="24"/>
+      <c r="FE71" s="24"/>
+      <c r="FF71" s="24"/>
+      <c r="FG71" s="24"/>
+      <c r="FH71" s="24"/>
     </row>
     <row r="72" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B72" s="25" t="s">
         <v>191</v>
@@ -18158,16 +18297,16 @@
         <v>216</v>
       </c>
       <c r="W72" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X72" s="20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Y72" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z72" s="20" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="AA72" s="20" t="s">
         <v>3</v>
@@ -18175,7 +18314,7 @@
     </row>
     <row r="73" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B73" s="25" t="s">
         <v>191</v>
@@ -18241,10 +18380,10 @@
         <v>216</v>
       </c>
       <c r="W73" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="X73" s="20" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="Y73" s="20" t="s">
         <v>2</v>
@@ -18257,143 +18396,87 @@
       </c>
     </row>
     <row r="74" spans="1:164" x14ac:dyDescent="0.2">
-      <c r="AB74" s="24"/>
-      <c r="AC74" s="24"/>
-      <c r="AD74" s="24"/>
-      <c r="AE74" s="24"/>
-      <c r="AF74" s="24"/>
-      <c r="AG74" s="24"/>
-      <c r="AH74" s="24"/>
-      <c r="AI74" s="24"/>
-      <c r="AJ74" s="24"/>
-      <c r="AK74" s="24"/>
-      <c r="AL74" s="24"/>
-      <c r="AM74" s="24"/>
-      <c r="AN74" s="24"/>
-      <c r="AO74" s="24"/>
-      <c r="AP74" s="24"/>
-      <c r="AQ74" s="24"/>
-      <c r="AR74" s="24"/>
-      <c r="AS74" s="24"/>
-      <c r="AT74" s="24"/>
-      <c r="AU74" s="24"/>
-      <c r="AV74" s="24"/>
-      <c r="AW74" s="24"/>
-      <c r="AX74" s="24"/>
-      <c r="AY74" s="24"/>
-      <c r="AZ74" s="24"/>
-      <c r="BA74" s="24"/>
-      <c r="BB74" s="24"/>
-      <c r="BC74" s="24"/>
-      <c r="BD74" s="24"/>
-      <c r="BE74" s="24"/>
-      <c r="BF74" s="24"/>
-      <c r="BG74" s="24"/>
-      <c r="BH74" s="24"/>
-      <c r="BI74" s="24"/>
-      <c r="BJ74" s="24"/>
-      <c r="BK74" s="24"/>
-      <c r="BL74" s="24"/>
-      <c r="BM74" s="24"/>
-      <c r="BN74" s="24"/>
-      <c r="BO74" s="24"/>
-      <c r="BP74" s="24"/>
-      <c r="BQ74" s="24"/>
-      <c r="BR74" s="24"/>
-      <c r="BS74" s="24"/>
-      <c r="BT74" s="24"/>
-      <c r="BU74" s="24"/>
-      <c r="BV74" s="24"/>
-      <c r="BW74" s="24"/>
-      <c r="BX74" s="24"/>
-      <c r="BY74" s="24"/>
-      <c r="BZ74" s="24"/>
-      <c r="CA74" s="24"/>
-      <c r="CB74" s="24"/>
-      <c r="CC74" s="24"/>
-      <c r="CD74" s="24"/>
-      <c r="CE74" s="24"/>
-      <c r="CF74" s="24"/>
-      <c r="CG74" s="24"/>
-      <c r="CH74" s="24"/>
-      <c r="CI74" s="24"/>
-      <c r="CJ74" s="24"/>
-      <c r="CK74" s="24"/>
-      <c r="CL74" s="24"/>
-      <c r="CM74" s="24"/>
-      <c r="CN74" s="24"/>
-      <c r="CO74" s="24"/>
-      <c r="CP74" s="24"/>
-      <c r="CQ74" s="24"/>
-      <c r="CR74" s="24"/>
-      <c r="CS74" s="24"/>
-      <c r="CT74" s="24"/>
-      <c r="CU74" s="24"/>
-      <c r="CV74" s="24"/>
-      <c r="CW74" s="24"/>
-      <c r="CX74" s="24"/>
-      <c r="CY74" s="24"/>
-      <c r="CZ74" s="24"/>
-      <c r="DA74" s="24"/>
-      <c r="DB74" s="24"/>
-      <c r="DC74" s="24"/>
-      <c r="DD74" s="24"/>
-      <c r="DE74" s="24"/>
-      <c r="DF74" s="24"/>
-      <c r="DG74" s="24"/>
-      <c r="DH74" s="24"/>
-      <c r="DI74" s="24"/>
-      <c r="DJ74" s="24"/>
-      <c r="DK74" s="24"/>
-      <c r="DL74" s="24"/>
-      <c r="DM74" s="24"/>
-      <c r="DN74" s="24"/>
-      <c r="DO74" s="24"/>
-      <c r="DP74" s="24"/>
-      <c r="DQ74" s="24"/>
-      <c r="DR74" s="24"/>
-      <c r="DS74" s="24"/>
-      <c r="DT74" s="24"/>
-      <c r="DU74" s="24"/>
-      <c r="DV74" s="24"/>
-      <c r="DW74" s="24"/>
-      <c r="DX74" s="24"/>
-      <c r="DY74" s="24"/>
-      <c r="DZ74" s="24"/>
-      <c r="EA74" s="24"/>
-      <c r="EB74" s="24"/>
-      <c r="EC74" s="24"/>
-      <c r="ED74" s="24"/>
-      <c r="EE74" s="24"/>
-      <c r="EF74" s="24"/>
-      <c r="EG74" s="24"/>
-      <c r="EH74" s="24"/>
-      <c r="EI74" s="24"/>
-      <c r="EJ74" s="24"/>
-      <c r="EK74" s="24"/>
-      <c r="EL74" s="24"/>
-      <c r="EM74" s="24"/>
-      <c r="EN74" s="24"/>
-      <c r="EO74" s="24"/>
-      <c r="EP74" s="24"/>
-      <c r="EQ74" s="24"/>
-      <c r="ER74" s="24"/>
-      <c r="ES74" s="24"/>
-      <c r="ET74" s="24"/>
-      <c r="EU74" s="24"/>
-      <c r="EV74" s="24"/>
-      <c r="EW74" s="24"/>
-      <c r="EX74" s="24"/>
-      <c r="EY74" s="24"/>
-      <c r="EZ74" s="24"/>
-      <c r="FA74" s="24"/>
-      <c r="FB74" s="24"/>
-      <c r="FC74" s="24"/>
-      <c r="FD74" s="24"/>
-      <c r="FE74" s="24"/>
-      <c r="FF74" s="24"/>
-      <c r="FG74" s="24"/>
-      <c r="FH74" s="24"/>
+      <c r="A74" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C74" s="25">
+        <v>500</v>
+      </c>
+      <c r="D74" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F74" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G74" s="27">
+        <v>1</v>
+      </c>
+      <c r="H74" s="27">
+        <v>1</v>
+      </c>
+      <c r="I74" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="J74" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="K74" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="L74" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="M74" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="N74" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="O74" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="P74" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q74" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="R74" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S74" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T74" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U74" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V74" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="W74" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="X74" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y74" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z74" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AA74" s="20" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="75" spans="1:164" x14ac:dyDescent="0.2">
       <c r="AB75" s="24"/>
@@ -20063,9 +20146,148 @@
       <c r="FG86" s="24"/>
       <c r="FH86" s="24"/>
     </row>
+    <row r="87" spans="28:164" x14ac:dyDescent="0.2">
+      <c r="AB87" s="24"/>
+      <c r="AC87" s="24"/>
+      <c r="AD87" s="24"/>
+      <c r="AE87" s="24"/>
+      <c r="AF87" s="24"/>
+      <c r="AG87" s="24"/>
+      <c r="AH87" s="24"/>
+      <c r="AI87" s="24"/>
+      <c r="AJ87" s="24"/>
+      <c r="AK87" s="24"/>
+      <c r="AL87" s="24"/>
+      <c r="AM87" s="24"/>
+      <c r="AN87" s="24"/>
+      <c r="AO87" s="24"/>
+      <c r="AP87" s="24"/>
+      <c r="AQ87" s="24"/>
+      <c r="AR87" s="24"/>
+      <c r="AS87" s="24"/>
+      <c r="AT87" s="24"/>
+      <c r="AU87" s="24"/>
+      <c r="AV87" s="24"/>
+      <c r="AW87" s="24"/>
+      <c r="AX87" s="24"/>
+      <c r="AY87" s="24"/>
+      <c r="AZ87" s="24"/>
+      <c r="BA87" s="24"/>
+      <c r="BB87" s="24"/>
+      <c r="BC87" s="24"/>
+      <c r="BD87" s="24"/>
+      <c r="BE87" s="24"/>
+      <c r="BF87" s="24"/>
+      <c r="BG87" s="24"/>
+      <c r="BH87" s="24"/>
+      <c r="BI87" s="24"/>
+      <c r="BJ87" s="24"/>
+      <c r="BK87" s="24"/>
+      <c r="BL87" s="24"/>
+      <c r="BM87" s="24"/>
+      <c r="BN87" s="24"/>
+      <c r="BO87" s="24"/>
+      <c r="BP87" s="24"/>
+      <c r="BQ87" s="24"/>
+      <c r="BR87" s="24"/>
+      <c r="BS87" s="24"/>
+      <c r="BT87" s="24"/>
+      <c r="BU87" s="24"/>
+      <c r="BV87" s="24"/>
+      <c r="BW87" s="24"/>
+      <c r="BX87" s="24"/>
+      <c r="BY87" s="24"/>
+      <c r="BZ87" s="24"/>
+      <c r="CA87" s="24"/>
+      <c r="CB87" s="24"/>
+      <c r="CC87" s="24"/>
+      <c r="CD87" s="24"/>
+      <c r="CE87" s="24"/>
+      <c r="CF87" s="24"/>
+      <c r="CG87" s="24"/>
+      <c r="CH87" s="24"/>
+      <c r="CI87" s="24"/>
+      <c r="CJ87" s="24"/>
+      <c r="CK87" s="24"/>
+      <c r="CL87" s="24"/>
+      <c r="CM87" s="24"/>
+      <c r="CN87" s="24"/>
+      <c r="CO87" s="24"/>
+      <c r="CP87" s="24"/>
+      <c r="CQ87" s="24"/>
+      <c r="CR87" s="24"/>
+      <c r="CS87" s="24"/>
+      <c r="CT87" s="24"/>
+      <c r="CU87" s="24"/>
+      <c r="CV87" s="24"/>
+      <c r="CW87" s="24"/>
+      <c r="CX87" s="24"/>
+      <c r="CY87" s="24"/>
+      <c r="CZ87" s="24"/>
+      <c r="DA87" s="24"/>
+      <c r="DB87" s="24"/>
+      <c r="DC87" s="24"/>
+      <c r="DD87" s="24"/>
+      <c r="DE87" s="24"/>
+      <c r="DF87" s="24"/>
+      <c r="DG87" s="24"/>
+      <c r="DH87" s="24"/>
+      <c r="DI87" s="24"/>
+      <c r="DJ87" s="24"/>
+      <c r="DK87" s="24"/>
+      <c r="DL87" s="24"/>
+      <c r="DM87" s="24"/>
+      <c r="DN87" s="24"/>
+      <c r="DO87" s="24"/>
+      <c r="DP87" s="24"/>
+      <c r="DQ87" s="24"/>
+      <c r="DR87" s="24"/>
+      <c r="DS87" s="24"/>
+      <c r="DT87" s="24"/>
+      <c r="DU87" s="24"/>
+      <c r="DV87" s="24"/>
+      <c r="DW87" s="24"/>
+      <c r="DX87" s="24"/>
+      <c r="DY87" s="24"/>
+      <c r="DZ87" s="24"/>
+      <c r="EA87" s="24"/>
+      <c r="EB87" s="24"/>
+      <c r="EC87" s="24"/>
+      <c r="ED87" s="24"/>
+      <c r="EE87" s="24"/>
+      <c r="EF87" s="24"/>
+      <c r="EG87" s="24"/>
+      <c r="EH87" s="24"/>
+      <c r="EI87" s="24"/>
+      <c r="EJ87" s="24"/>
+      <c r="EK87" s="24"/>
+      <c r="EL87" s="24"/>
+      <c r="EM87" s="24"/>
+      <c r="EN87" s="24"/>
+      <c r="EO87" s="24"/>
+      <c r="EP87" s="24"/>
+      <c r="EQ87" s="24"/>
+      <c r="ER87" s="24"/>
+      <c r="ES87" s="24"/>
+      <c r="ET87" s="24"/>
+      <c r="EU87" s="24"/>
+      <c r="EV87" s="24"/>
+      <c r="EW87" s="24"/>
+      <c r="EX87" s="24"/>
+      <c r="EY87" s="24"/>
+      <c r="EZ87" s="24"/>
+      <c r="FA87" s="24"/>
+      <c r="FB87" s="24"/>
+      <c r="FC87" s="24"/>
+      <c r="FD87" s="24"/>
+      <c r="FE87" s="24"/>
+      <c r="FF87" s="24"/>
+      <c r="FG87" s="24"/>
+      <c r="FH87" s="24"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA73">
-    <sortCondition ref="C2:C73"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA74">
+    <sortCondition ref="C2:C74"/>
   </sortState>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Validating complete build (all except proto-eve)
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEDC208-F965-464A-85A1-39BE37CA9B7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E7D1EB-9441-F242-8C30-7EE137F22435}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11040" yWindow="1100" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="293">
   <si>
     <t>virus_subfamily</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>source_name</t>
-  </si>
-  <si>
-    <t>Herpesvirus</t>
   </si>
   <si>
     <t>Dependo_B</t>
@@ -3408,10 +3405,10 @@
   <dimension ref="A1:FH97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P81" sqref="P81"/>
+      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3450,34 +3447,34 @@
         <v>74</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>97</v>
@@ -3533,7 +3530,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="25">
         <v>0</v>
@@ -3542,10 +3539,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G2" s="27">
         <v>1</v>
@@ -3554,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>129</v>
@@ -3603,7 +3600,7 @@
         <v>2</v>
       </c>
       <c r="Z2" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA2" s="20" t="s">
         <v>3</v>
@@ -3614,7 +3611,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="25">
         <v>1</v>
@@ -3626,7 +3623,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G3" s="25">
         <v>23</v>
@@ -3635,7 +3632,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>130</v>
@@ -3686,7 +3683,7 @@
         <v>2</v>
       </c>
       <c r="Z3" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA3" s="20" t="s">
         <v>3</v>
@@ -3694,10 +3691,10 @@
     </row>
     <row r="4" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="25">
         <v>2</v>
@@ -3709,7 +3706,7 @@
         <v>127</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G4" s="25">
         <v>8</v>
@@ -3718,7 +3715,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>129</v>
@@ -3736,7 +3733,7 @@
         <v>129</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>84</v>
@@ -3758,16 +3755,16 @@
         <v>32913662</v>
       </c>
       <c r="W4" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z4" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA4" s="20" t="s">
         <v>3</v>
@@ -3778,7 +3775,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C5" s="25">
         <v>3</v>
@@ -3790,7 +3787,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G5" s="25">
         <v>3</v>
@@ -3799,7 +3796,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>129</v>
@@ -3817,7 +3814,7 @@
         <v>129</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>84</v>
@@ -3850,7 +3847,7 @@
         <v>2</v>
       </c>
       <c r="Z5" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA5" s="20" t="s">
         <v>3</v>
@@ -3998,7 +3995,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" s="25">
         <v>4</v>
@@ -4010,7 +4007,7 @@
         <v>109</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G6" s="27">
         <v>4</v>
@@ -4019,7 +4016,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>130</v>
@@ -4058,7 +4055,7 @@
         <v>27.9</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W6" s="20" t="s">
         <v>111</v>
@@ -4070,7 +4067,7 @@
         <v>2</v>
       </c>
       <c r="Z6" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA6" s="20" t="s">
         <v>3</v>
@@ -4218,7 +4215,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="25">
         <v>5</v>
@@ -4230,7 +4227,7 @@
         <v>109</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G7" s="27">
         <v>4</v>
@@ -4239,13 +4236,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>22</v>
@@ -4257,7 +4254,7 @@
         <v>129</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>84</v>
@@ -4278,7 +4275,7 @@
         <v>27.9</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W7" s="20" t="s">
         <v>110</v>
@@ -4290,7 +4287,7 @@
         <v>2</v>
       </c>
       <c r="Z7" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA7" s="20" t="s">
         <v>3</v>
@@ -4438,7 +4435,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="25">
         <v>6</v>
@@ -4447,10 +4444,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G8" s="25">
         <v>1</v>
@@ -4459,19 +4456,19 @@
         <v>1</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N8" s="14" t="s">
         <v>22</v>
@@ -4496,7 +4493,7 @@
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W8" s="20" t="s">
         <v>9</v>
@@ -4508,7 +4505,7 @@
         <v>2</v>
       </c>
       <c r="Z8" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA8" s="20" t="s">
         <v>3</v>
@@ -4656,7 +4653,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C9" s="25">
         <v>7</v>
@@ -4668,7 +4665,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G9" s="25">
         <v>1</v>
@@ -4677,19 +4674,19 @@
         <v>1</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>22</v>
@@ -4714,7 +4711,7 @@
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W9" s="20" t="s">
         <v>10</v>
@@ -4726,7 +4723,7 @@
         <v>2</v>
       </c>
       <c r="Z9" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA9" s="20" t="s">
         <v>3</v>
@@ -4874,7 +4871,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C10" s="25">
         <v>8</v>
@@ -4886,7 +4883,7 @@
         <v>89</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G10" s="25">
         <v>1</v>
@@ -4895,13 +4892,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K10" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L10" s="14" t="s">
         <v>22</v>
@@ -4913,7 +4910,7 @@
         <v>129</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P10" s="4" t="s">
         <v>84</v>
@@ -4932,7 +4929,7 @@
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W10" s="20" t="s">
         <v>11</v>
@@ -4944,7 +4941,7 @@
         <v>2</v>
       </c>
       <c r="Z10" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA10" s="20" t="s">
         <v>3</v>
@@ -5089,10 +5086,10 @@
     </row>
     <row r="11" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="25">
         <v>9</v>
@@ -5101,10 +5098,10 @@
         <v>83</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G11" s="25">
         <v>2</v>
@@ -5113,19 +5110,19 @@
         <v>2</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N11" s="14" t="s">
         <v>22</v>
@@ -5150,19 +5147,19 @@
       </c>
       <c r="U11" s="7"/>
       <c r="V11" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W11" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X11" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Y11" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z11" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA11" s="20" t="s">
         <v>3</v>
@@ -5310,7 +5307,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C12" s="25">
         <v>10</v>
@@ -5322,7 +5319,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G12" s="27">
         <v>1</v>
@@ -5368,7 +5365,7 @@
       </c>
       <c r="U12" s="7"/>
       <c r="V12" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W12" s="20" t="s">
         <v>39</v>
@@ -5380,7 +5377,7 @@
         <v>2</v>
       </c>
       <c r="Z12" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA12" s="20" t="s">
         <v>3</v>
@@ -5528,7 +5525,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C13" s="25">
         <v>11</v>
@@ -5540,7 +5537,7 @@
         <v>122</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G13" s="27">
         <v>3</v>
@@ -5555,13 +5552,13 @@
         <v>129</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N13" s="14" t="s">
         <v>22</v>
@@ -5586,7 +5583,7 @@
       </c>
       <c r="U13" s="7"/>
       <c r="V13" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W13" s="20" t="s">
         <v>12</v>
@@ -5598,7 +5595,7 @@
         <v>2</v>
       </c>
       <c r="Z13" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA13" s="20" t="s">
         <v>3</v>
@@ -5746,7 +5743,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C14" s="25">
         <v>12</v>
@@ -5758,7 +5755,7 @@
         <v>86</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G14" s="25">
         <v>1</v>
@@ -5767,7 +5764,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>129</v>
@@ -5785,7 +5782,7 @@
         <v>129</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P14" s="3" t="s">
         <v>84</v>
@@ -5804,7 +5801,7 @@
       </c>
       <c r="U14" s="7"/>
       <c r="V14" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W14" s="20" t="s">
         <v>65</v>
@@ -5816,7 +5813,7 @@
         <v>2</v>
       </c>
       <c r="Z14" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA14" s="20" t="s">
         <v>3</v>
@@ -5964,7 +5961,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C15" s="25">
         <v>13</v>
@@ -5976,7 +5973,7 @@
         <v>87</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G15" s="27">
         <v>3</v>
@@ -5985,25 +5982,25 @@
         <v>3</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L15" s="13" t="s">
         <v>129</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N15" s="13" t="s">
         <v>129</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P15" s="17" t="s">
         <v>114</v>
@@ -6024,7 +6021,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W15" s="20" t="s">
         <v>8</v>
@@ -6036,7 +6033,7 @@
         <v>2</v>
       </c>
       <c r="Z15" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA15" s="20" t="s">
         <v>3</v>
@@ -6184,7 +6181,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C16" s="25">
         <v>14</v>
@@ -6196,7 +6193,7 @@
         <v>87</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G16" s="27">
         <v>5</v>
@@ -6205,19 +6202,19 @@
         <v>5</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N16" s="14" t="s">
         <v>22</v>
@@ -6244,7 +6241,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W16" s="20" t="s">
         <v>27</v>
@@ -6256,7 +6253,7 @@
         <v>2</v>
       </c>
       <c r="Z16" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA16" s="20" t="s">
         <v>3</v>
@@ -6404,7 +6401,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C17" s="25">
         <v>15</v>
@@ -6416,7 +6413,7 @@
         <v>106</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G17" s="27">
         <v>1</v>
@@ -6425,19 +6422,19 @@
         <v>1</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N17" s="14" t="s">
         <v>22</v>
@@ -6464,7 +6461,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W17" s="20" t="s">
         <v>80</v>
@@ -6476,7 +6473,7 @@
         <v>2</v>
       </c>
       <c r="Z17" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA17" s="20" t="s">
         <v>3</v>
@@ -6624,7 +6621,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C18" s="25">
         <v>16</v>
@@ -6636,7 +6633,7 @@
         <v>90</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G18" s="27">
         <v>5</v>
@@ -6645,7 +6642,7 @@
         <v>5</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>130</v>
@@ -6682,7 +6679,7 @@
       </c>
       <c r="U18" s="8"/>
       <c r="V18" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W18" s="20" t="s">
         <v>75</v>
@@ -6694,7 +6691,7 @@
         <v>2</v>
       </c>
       <c r="Z18" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA18" s="20" t="s">
         <v>3</v>
@@ -6842,7 +6839,7 @@
         <v>126</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C19" s="25">
         <v>20</v>
@@ -6854,7 +6851,7 @@
         <v>82</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G19" s="27">
         <v>13</v>
@@ -6863,7 +6860,7 @@
         <v>13</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>131</v>
@@ -6900,7 +6897,7 @@
       </c>
       <c r="U19" s="8"/>
       <c r="V19" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W19" s="20" t="s">
         <v>126</v>
@@ -6912,7 +6909,7 @@
         <v>2</v>
       </c>
       <c r="Z19" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA19" s="20" t="s">
         <v>3</v>
@@ -7060,7 +7057,7 @@
         <v>81</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C20" s="25">
         <v>22</v>
@@ -7072,7 +7069,7 @@
         <v>82</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G20" s="27">
         <v>73</v>
@@ -7081,7 +7078,7 @@
         <v>76</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>131</v>
@@ -7120,7 +7117,7 @@
         <v>62</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W20" s="20" t="s">
         <v>81</v>
@@ -7132,7 +7129,7 @@
         <v>2</v>
       </c>
       <c r="Z20" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA20" s="20" t="s">
         <v>3</v>
@@ -7277,10 +7274,10 @@
     </row>
     <row r="21" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C21" s="25">
         <v>23</v>
@@ -7292,7 +7289,7 @@
         <v>91</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G21" s="27">
         <v>5</v>
@@ -7301,7 +7298,7 @@
         <v>5</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>130</v>
@@ -7343,16 +7340,16 @@
         <v>26037535</v>
       </c>
       <c r="W21" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X21" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y21" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z21" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA21" s="20" t="s">
         <v>3</v>
@@ -7497,22 +7494,22 @@
     </row>
     <row r="22" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C22" s="25">
         <v>26</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G22" s="27">
         <v>7</v>
@@ -7521,7 +7518,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>130</v>
@@ -7563,16 +7560,16 @@
         <v>15085543</v>
       </c>
       <c r="W22" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="X22" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="Y22" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z22" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA22" s="20" t="s">
         <v>3</v>
@@ -7720,7 +7717,7 @@
         <v>64</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C23" s="25">
         <v>27</v>
@@ -7732,7 +7729,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G23" s="27">
         <v>3</v>
@@ -7741,19 +7738,19 @@
         <v>3</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J23" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N23" s="14" t="s">
         <v>22</v>
@@ -7778,7 +7775,7 @@
       </c>
       <c r="U23" s="8"/>
       <c r="V23" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W23" s="20" t="s">
         <v>64</v>
@@ -7790,7 +7787,7 @@
         <v>2</v>
       </c>
       <c r="Z23" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA23" s="20" t="s">
         <v>3</v>
@@ -7938,7 +7935,7 @@
         <v>78</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C24" s="25">
         <v>28</v>
@@ -7950,7 +7947,7 @@
         <v>93</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="27">
         <v>1</v>
@@ -7959,7 +7956,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>130</v>
@@ -7986,17 +7983,17 @@
         <v>117</v>
       </c>
       <c r="R24" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>224</v>
       </c>
       <c r="T24" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U24" s="8"/>
       <c r="V24" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W24" s="20" t="s">
         <v>78</v>
@@ -8008,7 +8005,7 @@
         <v>2</v>
       </c>
       <c r="Z24" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA24" s="20" t="s">
         <v>3</v>
@@ -8153,10 +8150,10 @@
     </row>
     <row r="25" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="25">
         <v>36</v>
@@ -8168,7 +8165,7 @@
         <v>121</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G25" s="27">
         <v>1</v>
@@ -8204,29 +8201,29 @@
         <v>117</v>
       </c>
       <c r="R25" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>177</v>
-      </c>
-      <c r="S25" s="10" t="s">
-        <v>178</v>
       </c>
       <c r="T25" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U25" s="8"/>
       <c r="V25" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W25" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="X25" s="20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="Y25" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z25" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA25" s="20" t="s">
         <v>3</v>
@@ -8371,10 +8368,10 @@
     </row>
     <row r="26" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C26" s="25">
         <v>37</v>
@@ -8383,10 +8380,10 @@
         <v>20</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G26" s="25">
         <v>1</v>
@@ -8395,25 +8392,25 @@
         <v>1</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>129</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P26" s="3" t="s">
         <v>84</v>
@@ -8422,29 +8419,29 @@
         <v>117</v>
       </c>
       <c r="R26" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="S26" s="10" t="s">
         <v>225</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="T26" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U26" s="8"/>
       <c r="V26" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W26" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X26" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y26" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z26" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA26" s="20" t="s">
         <v>3</v>
@@ -8592,7 +8589,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C27" s="25">
         <v>40</v>
@@ -8604,7 +8601,7 @@
         <v>119</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G27" s="27">
         <v>1</v>
@@ -8613,7 +8610,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>130</v>
@@ -8640,11 +8637,11 @@
         <v>117</v>
       </c>
       <c r="R27" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="S27" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="S27" s="10" t="s">
-        <v>236</v>
-      </c>
       <c r="T27" s="8" t="s">
         <v>43</v>
       </c>
@@ -8652,7 +8649,7 @@
         <v>43</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W27" s="20" t="s">
         <v>120</v>
@@ -8664,7 +8661,7 @@
         <v>2</v>
       </c>
       <c r="Z27" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA27" s="20" t="s">
         <v>3</v>
@@ -8812,7 +8809,7 @@
         <v>124</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C28" s="25">
         <v>42</v>
@@ -8824,7 +8821,7 @@
         <v>96</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G28" s="25">
         <v>1</v>
@@ -8833,19 +8830,19 @@
         <v>1</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K28" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L28" s="13" t="s">
         <v>129</v>
       </c>
       <c r="M28" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N28" s="14" t="s">
         <v>22</v>
@@ -8870,7 +8867,7 @@
       </c>
       <c r="U28" s="7"/>
       <c r="V28" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W28" s="20" t="s">
         <v>124</v>
@@ -8882,7 +8879,7 @@
         <v>2</v>
       </c>
       <c r="Z28" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA28" s="20" t="s">
         <v>3</v>
@@ -9030,7 +9027,7 @@
         <v>123</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C29" s="25">
         <v>43</v>
@@ -9042,7 +9039,7 @@
         <v>125</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G29" s="25">
         <v>5</v>
@@ -9051,7 +9048,7 @@
         <v>5</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>129</v>
@@ -9088,7 +9085,7 @@
       </c>
       <c r="U29" s="8"/>
       <c r="V29" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W29" s="20" t="s">
         <v>123</v>
@@ -9100,7 +9097,7 @@
         <v>2</v>
       </c>
       <c r="Z29" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA29" s="20" t="s">
         <v>3</v>
@@ -9260,7 +9257,7 @@
         <v>104</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G30" s="27">
         <v>2</v>
@@ -9308,7 +9305,7 @@
         <v>34</v>
       </c>
       <c r="V30" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W30" s="20" t="s">
         <v>25</v>
@@ -9320,7 +9317,7 @@
         <v>2</v>
       </c>
       <c r="Z30" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA30" s="20" t="s">
         <v>3</v>
@@ -9465,7 +9462,7 @@
     </row>
     <row r="31" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>84</v>
@@ -9480,7 +9477,7 @@
         <v>104</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G31" s="27">
         <v>2</v>
@@ -9526,19 +9523,19 @@
       </c>
       <c r="U31" s="8"/>
       <c r="V31" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W31" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="X31" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Y31" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z31" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA31" s="20" t="s">
         <v>3</v>
@@ -9683,10 +9680,10 @@
     </row>
     <row r="32" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C32" s="25">
         <v>46</v>
@@ -9698,7 +9695,7 @@
         <v>17</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G32" s="25">
         <v>1</v>
@@ -9707,25 +9704,25 @@
         <v>2</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>129</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L32" s="3" t="s">
         <v>129</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>129</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P32" s="3" t="s">
         <v>84</v>
@@ -9744,19 +9741,19 @@
       </c>
       <c r="U32" s="8"/>
       <c r="V32" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W32" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X32" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y32" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z32" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA32" s="20" t="s">
         <v>3</v>
@@ -9901,10 +9898,10 @@
     </row>
     <row r="33" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C33" s="25">
         <v>47</v>
@@ -9913,10 +9910,10 @@
         <v>15</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G33" s="27">
         <v>1</v>
@@ -9952,11 +9949,11 @@
         <v>117</v>
       </c>
       <c r="R33" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="S33" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="S33" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="T33" s="8" t="s">
         <v>43</v>
       </c>
@@ -9964,19 +9961,19 @@
         <v>43</v>
       </c>
       <c r="V33" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W33" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="X33" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Y33" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z33" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA33" s="20" t="s">
         <v>3</v>
@@ -10121,10 +10118,10 @@
     </row>
     <row r="34" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C34" s="25">
         <v>48</v>
@@ -10136,7 +10133,7 @@
         <v>105</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>117</v>
@@ -10151,13 +10148,13 @@
         <v>129</v>
       </c>
       <c r="K34" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L34" s="13" t="s">
         <v>129</v>
       </c>
       <c r="M34" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>43</v>
@@ -10182,19 +10179,19 @@
       </c>
       <c r="U34" s="8"/>
       <c r="V34" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W34" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="X34" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y34" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z34" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA34" s="20" t="s">
         <v>3</v>
@@ -10339,10 +10336,10 @@
     </row>
     <row r="35" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C35" s="25">
         <v>49</v>
@@ -10351,7 +10348,7 @@
         <v>15</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>117</v>
@@ -10400,19 +10397,19 @@
       </c>
       <c r="U35" s="8"/>
       <c r="V35" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W35" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="X35" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Y35" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z35" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA35" s="20" t="s">
         <v>3</v>
@@ -10557,10 +10554,10 @@
     </row>
     <row r="36" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C36" s="25">
         <v>50</v>
@@ -10569,7 +10566,7 @@
         <v>21</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>117</v>
@@ -10608,29 +10605,29 @@
         <v>117</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="T36" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U36" s="8"/>
       <c r="V36" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W36" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X36" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y36" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z36" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA36" s="20" t="s">
         <v>3</v>
@@ -10778,7 +10775,7 @@
         <v>128</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C37" s="25">
         <v>51</v>
@@ -10787,10 +10784,10 @@
         <v>21</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G37" s="25">
         <v>4</v>
@@ -10826,17 +10823,17 @@
         <v>117</v>
       </c>
       <c r="R37" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="S37" s="10" t="s">
         <v>183</v>
-      </c>
-      <c r="S37" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="T37" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U37" s="8"/>
       <c r="V37" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W37" s="20" t="s">
         <v>128</v>
@@ -10848,7 +10845,7 @@
         <v>2</v>
       </c>
       <c r="Z37" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA37" s="20" t="s">
         <v>3</v>
@@ -10993,10 +10990,10 @@
     </row>
     <row r="38" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C38" s="25">
         <v>54</v>
@@ -11005,10 +11002,10 @@
         <v>20</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G38" s="27">
         <v>3</v>
@@ -11054,19 +11051,19 @@
       </c>
       <c r="U38" s="8"/>
       <c r="V38" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W38" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="X38" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y38" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z38" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA38" s="20" t="s">
         <v>3</v>
@@ -11211,10 +11208,10 @@
     </row>
     <row r="39" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C39" s="25">
         <v>55</v>
@@ -11226,7 +11223,7 @@
         <v>17</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G39" s="25" t="s">
         <v>117</v>
@@ -11272,19 +11269,19 @@
       </c>
       <c r="U39" s="8"/>
       <c r="V39" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W39" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X39" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y39" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z39" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA39" s="20" t="s">
         <v>3</v>
@@ -11429,10 +11426,10 @@
     </row>
     <row r="40" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C40" s="25">
         <v>56</v>
@@ -11444,7 +11441,7 @@
         <v>107</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G40" s="27">
         <v>3</v>
@@ -11453,7 +11450,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>129</v>
@@ -11489,19 +11486,19 @@
         <v>43</v>
       </c>
       <c r="V40" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W40" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X40" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y40" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z40" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA40" s="20" t="s">
         <v>3</v>
@@ -11646,10 +11643,10 @@
     </row>
     <row r="41" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C41" s="25">
         <v>58</v>
@@ -11658,7 +11655,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F41" s="22" t="s">
         <v>117</v>
@@ -11707,19 +11704,19 @@
       </c>
       <c r="U41" s="8"/>
       <c r="V41" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W41" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="X41" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Y41" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z41" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA41" s="20" t="s">
         <v>3</v>
@@ -11864,10 +11861,10 @@
     </row>
     <row r="42" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C42" s="25">
         <v>59</v>
@@ -11876,7 +11873,7 @@
         <v>83</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F42" s="22" t="s">
         <v>117</v>
@@ -11915,28 +11912,28 @@
         <v>117</v>
       </c>
       <c r="R42" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S42" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T42" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V42" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W42" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="X42" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Y42" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z42" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA42" s="20" t="s">
         <v>3</v>
@@ -12081,10 +12078,10 @@
     </row>
     <row r="43" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C43" s="25">
         <v>60</v>
@@ -12093,10 +12090,10 @@
         <v>15</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G43" s="29">
         <v>1</v>
@@ -12144,19 +12141,19 @@
         <v>43</v>
       </c>
       <c r="V43" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W43" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="X43" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y43" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z43" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA43" s="20" t="s">
         <v>3</v>
@@ -12301,10 +12298,10 @@
     </row>
     <row r="44" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C44" s="25">
         <v>61</v>
@@ -12313,10 +12310,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G44" s="29">
         <v>1</v>
@@ -12364,19 +12361,19 @@
         <v>43</v>
       </c>
       <c r="V44" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W44" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X44" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Y44" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z44" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA44" s="20" t="s">
         <v>3</v>
@@ -12521,10 +12518,10 @@
     </row>
     <row r="45" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C45" s="25">
         <v>62</v>
@@ -12533,10 +12530,10 @@
         <v>15</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G45" s="29">
         <v>1</v>
@@ -12584,19 +12581,19 @@
         <v>43</v>
       </c>
       <c r="V45" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W45" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X45" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Y45" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z45" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA45" s="20" t="s">
         <v>3</v>
@@ -12741,10 +12738,10 @@
     </row>
     <row r="46" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C46" s="25">
         <v>63</v>
@@ -12792,11 +12789,11 @@
         <v>116</v>
       </c>
       <c r="R46" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="S46" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="S46" s="10" t="s">
-        <v>195</v>
-      </c>
       <c r="T46" s="8" t="s">
         <v>43</v>
       </c>
@@ -12804,19 +12801,19 @@
         <v>43</v>
       </c>
       <c r="V46" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W46" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="X46" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Y46" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z46" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA46" s="20" t="s">
         <v>3</v>
@@ -12961,10 +12958,10 @@
     </row>
     <row r="47" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C47" s="25">
         <v>64</v>
@@ -13022,19 +13019,19 @@
       </c>
       <c r="U47" s="8"/>
       <c r="V47" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W47" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X47" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Y47" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z47" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA47" s="20" t="s">
         <v>3</v>
@@ -13179,10 +13176,10 @@
     </row>
     <row r="48" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C48" s="25">
         <v>75</v>
@@ -13191,7 +13188,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>117</v>
@@ -13240,19 +13237,19 @@
       </c>
       <c r="U48" s="8"/>
       <c r="V48" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W48" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="X48" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Y48" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z48" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA48" s="20" t="s">
         <v>3</v>
@@ -13397,10 +13394,10 @@
     </row>
     <row r="49" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C49" s="25">
         <v>76</v>
@@ -13409,7 +13406,7 @@
         <v>21</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>117</v>
@@ -13458,19 +13455,19 @@
       </c>
       <c r="U49" s="8"/>
       <c r="V49" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W49" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X49" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y49" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z49" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA49" s="20" t="s">
         <v>3</v>
@@ -13615,10 +13612,10 @@
     </row>
     <row r="50" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C50" s="25">
         <v>86</v>
@@ -13630,7 +13627,7 @@
         <v>119</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G50" s="25">
         <v>5</v>
@@ -13639,7 +13636,7 @@
         <v>5</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>130</v>
@@ -13666,11 +13663,11 @@
         <v>117</v>
       </c>
       <c r="R50" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="S50" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="S50" s="10" t="s">
-        <v>197</v>
-      </c>
       <c r="T50" s="8" t="s">
         <v>43</v>
       </c>
@@ -13678,19 +13675,19 @@
         <v>43</v>
       </c>
       <c r="V50" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W50" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="X50" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Y50" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z50" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA50" s="20" t="s">
         <v>3</v>
@@ -13835,10 +13832,10 @@
     </row>
     <row r="51" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C51" s="25">
         <v>87</v>
@@ -13847,7 +13844,7 @@
         <v>15</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>117</v>
@@ -13886,11 +13883,11 @@
         <v>117</v>
       </c>
       <c r="R51" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="S51" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="S51" s="10" t="s">
-        <v>240</v>
-      </c>
       <c r="T51" s="8" t="s">
         <v>43</v>
       </c>
@@ -13898,19 +13895,19 @@
         <v>43</v>
       </c>
       <c r="V51" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W51" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="X51" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Y51" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z51" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA51" s="20" t="s">
         <v>3</v>
@@ -14055,10 +14052,10 @@
     </row>
     <row r="52" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C52" s="25">
         <v>88</v>
@@ -14067,7 +14064,7 @@
         <v>15</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>117</v>
@@ -14102,31 +14099,31 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="33"/>
       <c r="R52" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="S52" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="T52" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U52" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V52" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="W52" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="S52" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="T52" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U52" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V52" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="W52" s="20" t="s">
-        <v>274</v>
-      </c>
       <c r="X52" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y52" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z52" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA52" s="20" t="s">
         <v>3</v>
@@ -14271,10 +14268,10 @@
     </row>
     <row r="53" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C53" s="25">
         <v>92</v>
@@ -14283,10 +14280,10 @@
         <v>15</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G53" s="27">
         <v>1</v>
@@ -14319,13 +14316,13 @@
         <v>84</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S53" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="T53" s="8" t="s">
         <v>43</v>
@@ -14334,19 +14331,19 @@
         <v>43</v>
       </c>
       <c r="V53" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W53" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X53" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y53" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z53" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA53" s="20" t="s">
         <v>3</v>
@@ -14491,10 +14488,10 @@
     </row>
     <row r="54" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C54" s="25">
         <v>100</v>
@@ -14503,7 +14500,7 @@
         <v>15</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F54" s="22" t="s">
         <v>117</v>
@@ -14542,29 +14539,29 @@
         <v>117</v>
       </c>
       <c r="R54" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S54" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="T54" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U54" s="8"/>
       <c r="V54" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W54" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="X54" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Y54" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z54" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA54" s="20" t="s">
         <v>3</v>
@@ -14709,10 +14706,10 @@
     </row>
     <row r="55" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C55" s="25">
         <v>160</v>
@@ -14724,7 +14721,7 @@
         <v>40</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G55" s="25">
         <v>1</v>
@@ -14733,7 +14730,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>129</v>
@@ -14757,31 +14754,31 @@
         <v>84</v>
       </c>
       <c r="Q55" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="T55" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V55" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="W55" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="W55" s="20" t="s">
-        <v>215</v>
-      </c>
       <c r="X55" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y55" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z55" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA55" s="20" t="s">
         <v>3</v>
@@ -14926,10 +14923,10 @@
     </row>
     <row r="56" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C56" s="25">
         <v>162</v>
@@ -14938,10 +14935,10 @@
         <v>15</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G56" s="27">
         <v>1</v>
@@ -14950,7 +14947,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>129</v>
@@ -14990,16 +14987,16 @@
         <v>27377618</v>
       </c>
       <c r="W56" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="X56" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y56" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z56" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA56" s="20" t="s">
         <v>3</v>
@@ -15144,10 +15141,10 @@
     </row>
     <row r="57" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C57" s="25">
         <v>163</v>
@@ -15156,10 +15153,10 @@
         <v>15</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G57" s="27">
         <v>1</v>
@@ -15168,7 +15165,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>129</v>
@@ -15208,16 +15205,16 @@
         <v>27377618</v>
       </c>
       <c r="W57" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="X57" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y57" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z57" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA57" s="20" t="s">
         <v>3</v>
@@ -15362,10 +15359,10 @@
     </row>
     <row r="58" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C58" s="25">
         <v>164</v>
@@ -15374,10 +15371,10 @@
         <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F58" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G58" s="27">
         <v>1</v>
@@ -15386,7 +15383,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>129</v>
@@ -15426,16 +15423,16 @@
         <v>27377618</v>
       </c>
       <c r="W58" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="X58" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Y58" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z58" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA58" s="20" t="s">
         <v>3</v>
@@ -15580,10 +15577,10 @@
     </row>
     <row r="59" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C59" s="25">
         <v>174</v>
@@ -15592,10 +15589,10 @@
         <v>15</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G59" s="27">
         <v>1</v>
@@ -15604,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>43</v>
@@ -15631,11 +15628,11 @@
         <v>117</v>
       </c>
       <c r="R59" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="S59" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="S59" s="10" t="s">
-        <v>176</v>
-      </c>
       <c r="T59" s="8" t="s">
         <v>43</v>
       </c>
@@ -15643,19 +15640,19 @@
         <v>43</v>
       </c>
       <c r="V59" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W59" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="X59" s="20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Y59" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z59" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA59" s="20" t="s">
         <v>3</v>
@@ -15800,10 +15797,10 @@
     </row>
     <row r="60" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C60" s="25">
         <v>175</v>
@@ -15812,7 +15809,7 @@
         <v>15</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F60" s="22" t="s">
         <v>117</v>
@@ -15861,19 +15858,19 @@
       </c>
       <c r="U60" s="8"/>
       <c r="V60" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W60" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X60" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y60" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z60" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA60" s="20" t="s">
         <v>3</v>
@@ -16018,10 +16015,10 @@
     </row>
     <row r="61" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C61" s="25">
         <v>176</v>
@@ -16030,7 +16027,7 @@
         <v>15</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F61" s="22" t="s">
         <v>117</v>
@@ -16079,19 +16076,19 @@
       </c>
       <c r="U61" s="8"/>
       <c r="V61" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W61" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="X61" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Y61" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z61" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA61" s="20" t="s">
         <v>3</v>
@@ -16236,10 +16233,10 @@
     </row>
     <row r="62" spans="1:164" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C62" s="25">
         <v>180</v>
@@ -16248,10 +16245,10 @@
         <v>15</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G62" s="27">
         <v>2</v>
@@ -16260,7 +16257,7 @@
         <v>2</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>43</v>
@@ -16287,11 +16284,11 @@
         <v>117</v>
       </c>
       <c r="R62" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="S62" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="S62" s="10" t="s">
-        <v>186</v>
-      </c>
       <c r="T62" s="8" t="s">
         <v>43</v>
       </c>
@@ -16299,19 +16296,19 @@
         <v>43</v>
       </c>
       <c r="V62" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W62" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="X62" s="20" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Y62" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z62" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA62" s="20" t="s">
         <v>3</v>
@@ -16456,10 +16453,10 @@
     </row>
     <row r="63" spans="1:164" s="26" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C63" s="25">
         <v>187</v>
@@ -16468,10 +16465,10 @@
         <v>15</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G63" s="25">
         <v>1</v>
@@ -16507,11 +16504,11 @@
         <v>117</v>
       </c>
       <c r="R63" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="S63" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="S63" s="10" t="s">
-        <v>233</v>
-      </c>
       <c r="T63" s="8" t="s">
         <v>43</v>
       </c>
@@ -16519,19 +16516,19 @@
         <v>43</v>
       </c>
       <c r="V63" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W63" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="X63" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y63" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z63" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA63" s="20" t="s">
         <v>3</v>
@@ -16676,10 +16673,10 @@
     </row>
     <row r="64" spans="1:164" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C64" s="25">
         <v>190</v>
@@ -16691,7 +16688,7 @@
         <v>40</v>
       </c>
       <c r="F64" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G64" s="25">
         <v>1</v>
@@ -16727,29 +16724,29 @@
         <v>117</v>
       </c>
       <c r="R64" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="S64" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="S64" s="10" t="s">
-        <v>243</v>
       </c>
       <c r="T64" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U64" s="7"/>
       <c r="V64" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W64" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X64" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y64" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z64" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA64" s="20" t="s">
         <v>3</v>
@@ -16894,10 +16891,10 @@
     </row>
     <row r="65" spans="1:164" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C65" s="25">
         <v>191</v>
@@ -16909,7 +16906,7 @@
         <v>40</v>
       </c>
       <c r="F65" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G65" s="25" t="s">
         <v>117</v>
@@ -16955,19 +16952,19 @@
       </c>
       <c r="U65" s="7"/>
       <c r="V65" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W65" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X65" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y65" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z65" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA65" s="20" t="s">
         <v>3</v>
@@ -17112,10 +17109,10 @@
     </row>
     <row r="66" spans="1:164" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C66" s="25">
         <v>192</v>
@@ -17127,7 +17124,7 @@
         <v>40</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G66" s="25" t="s">
         <v>117</v>
@@ -17172,19 +17169,19 @@
         <v>43</v>
       </c>
       <c r="V66" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W66" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="X66" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="Y66" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z66" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA66" s="20" t="s">
         <v>3</v>
@@ -17329,7 +17326,7 @@
     </row>
     <row r="67" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B67" s="25" t="s">
         <v>84</v>
@@ -17344,7 +17341,7 @@
         <v>94</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G67" s="29">
         <v>1</v>
@@ -17390,19 +17387,19 @@
       </c>
       <c r="U67" s="7"/>
       <c r="V67" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W67" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X67" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Y67" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z67" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA67" s="20" t="s">
         <v>3</v>
@@ -17547,7 +17544,7 @@
     </row>
     <row r="68" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B68" s="25" t="s">
         <v>84</v>
@@ -17562,7 +17559,7 @@
         <v>94</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G68" s="29">
         <v>1</v>
@@ -17607,19 +17604,19 @@
         <v>43</v>
       </c>
       <c r="V68" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W68" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X68" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y68" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z68" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA68" s="20" t="s">
         <v>3</v>
@@ -17764,7 +17761,7 @@
     </row>
     <row r="69" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>84</v>
@@ -17779,7 +17776,7 @@
         <v>94</v>
       </c>
       <c r="F69" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G69" s="29">
         <v>1</v>
@@ -17825,19 +17822,19 @@
       </c>
       <c r="U69" s="7"/>
       <c r="V69" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W69" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X69" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y69" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z69" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA69" s="20" t="s">
         <v>3</v>
@@ -17982,10 +17979,10 @@
     </row>
     <row r="70" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C70" s="25">
         <v>201</v>
@@ -17994,10 +17991,10 @@
         <v>15</v>
       </c>
       <c r="E70" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G70" s="27">
         <v>1</v>
@@ -18006,7 +18003,7 @@
         <v>1</v>
       </c>
       <c r="I70" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>43</v>
@@ -18033,31 +18030,31 @@
         <v>117</v>
       </c>
       <c r="R70" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="S70" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="S70" s="10" t="s">
+      <c r="T70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V70" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="W70" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="T70" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U70" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V70" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="W70" s="20" t="s">
-        <v>181</v>
-      </c>
       <c r="X70" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="Y70" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z70" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA70" s="20" t="s">
         <v>3</v>
@@ -18202,10 +18199,10 @@
     </row>
     <row r="71" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C71" s="25">
         <v>202</v>
@@ -18214,10 +18211,10 @@
         <v>15</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G71" s="27">
         <v>1</v>
@@ -18226,7 +18223,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>43</v>
@@ -18253,11 +18250,11 @@
         <v>117</v>
       </c>
       <c r="R71" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="S71" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="S71" s="10" t="s">
-        <v>180</v>
-      </c>
       <c r="T71" s="8" t="s">
         <v>43</v>
       </c>
@@ -18265,19 +18262,19 @@
         <v>43</v>
       </c>
       <c r="V71" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W71" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="X71" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y71" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z71" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA71" s="20" t="s">
         <v>3</v>
@@ -18422,10 +18419,10 @@
     </row>
     <row r="72" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C72" s="25">
         <v>203</v>
@@ -18434,10 +18431,10 @@
         <v>15</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F72" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G72" s="27">
         <v>1</v>
@@ -18485,19 +18482,19 @@
         <v>43</v>
       </c>
       <c r="V72" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W72" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X72" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Y72" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z72" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA72" s="20" t="s">
         <v>3</v>
@@ -18642,7 +18639,7 @@
     </row>
     <row r="73" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" s="25" t="s">
         <v>84</v>
@@ -18654,10 +18651,10 @@
         <v>15</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F73" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G73" s="27">
         <v>1</v>
@@ -18666,7 +18663,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>43</v>
@@ -18693,10 +18690,10 @@
         <v>117</v>
       </c>
       <c r="R73" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S73" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="T73" s="8" t="s">
         <v>43</v>
@@ -18705,19 +18702,19 @@
         <v>43</v>
       </c>
       <c r="V73" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W73" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="X73" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y73" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z73" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA73" s="20" t="s">
         <v>3</v>
@@ -18862,10 +18859,10 @@
     </row>
     <row r="74" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C74" s="25">
         <v>365</v>
@@ -18877,7 +18874,7 @@
         <v>95</v>
       </c>
       <c r="F74" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G74" s="25">
         <v>7</v>
@@ -18886,7 +18883,7 @@
         <v>7</v>
       </c>
       <c r="I74" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>43</v>
@@ -18913,10 +18910,10 @@
         <v>117</v>
       </c>
       <c r="R74" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S74" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T74" s="8" t="s">
         <v>43</v>
@@ -18925,19 +18922,19 @@
         <v>43</v>
       </c>
       <c r="V74" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W74" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X74" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Y74" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z74" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA74" s="20" t="s">
         <v>3</v>
@@ -18945,10 +18942,10 @@
     </row>
     <row r="75" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C75" s="25">
         <v>366</v>
@@ -18960,7 +18957,7 @@
         <v>95</v>
       </c>
       <c r="F75" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G75" s="25">
         <v>20</v>
@@ -18969,7 +18966,7 @@
         <v>20</v>
       </c>
       <c r="I75" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>43</v>
@@ -18996,10 +18993,10 @@
         <v>117</v>
       </c>
       <c r="R75" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="S75" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T75" s="8" t="s">
         <v>43</v>
@@ -19008,19 +19005,19 @@
         <v>43</v>
       </c>
       <c r="V75" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W75" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X75" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Y75" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z75" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA75" s="20" t="s">
         <v>3</v>
@@ -19165,10 +19162,10 @@
     </row>
     <row r="76" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C76" s="25">
         <v>367</v>
@@ -19177,10 +19174,10 @@
         <v>21</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F76" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G76" s="25" t="s">
         <v>117</v>
@@ -19224,19 +19221,19 @@
       </c>
       <c r="U76" s="7"/>
       <c r="V76" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W76" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="X76" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y76" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z76" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA76" s="20" t="s">
         <v>3</v>
@@ -19381,10 +19378,10 @@
     </row>
     <row r="77" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C77" s="25">
         <v>368</v>
@@ -19393,7 +19390,7 @@
         <v>21</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F77" s="22" t="s">
         <v>117</v>
@@ -19440,19 +19437,19 @@
       </c>
       <c r="U77" s="7"/>
       <c r="V77" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W77" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="X77" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Y77" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z77" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA77" s="20" t="s">
         <v>3</v>
@@ -19597,10 +19594,10 @@
     </row>
     <row r="78" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C78" s="25">
         <v>369</v>
@@ -19609,7 +19606,7 @@
         <v>15</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F78" s="22" t="s">
         <v>117</v>
@@ -19656,19 +19653,19 @@
       </c>
       <c r="U78" s="7"/>
       <c r="V78" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W78" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="X78" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Y78" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z78" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA78" s="20" t="s">
         <v>3</v>
@@ -19813,10 +19810,10 @@
     </row>
     <row r="79" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C79" s="25">
         <v>370</v>
@@ -19825,10 +19822,10 @@
         <v>15</v>
       </c>
       <c r="E79" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F79" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G79" s="27">
         <v>1</v>
@@ -19837,13 +19834,13 @@
         <v>1</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J79" s="13" t="s">
         <v>129</v>
       </c>
       <c r="K79" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>43</v>
@@ -19874,19 +19871,19 @@
       </c>
       <c r="U79" s="7"/>
       <c r="V79" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W79" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X79" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Y79" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z79" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA79" s="20" t="s">
         <v>3</v>
@@ -20031,10 +20028,10 @@
     </row>
     <row r="80" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C80" s="25">
         <v>371</v>
@@ -20043,10 +20040,10 @@
         <v>15</v>
       </c>
       <c r="E80" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F80" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G80" s="25" t="s">
         <v>117</v>
@@ -20090,19 +20087,19 @@
       </c>
       <c r="U80" s="7"/>
       <c r="V80" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W80" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="X80" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Y80" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z80" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA80" s="20" t="s">
         <v>3</v>
@@ -20247,10 +20244,10 @@
     </row>
     <row r="81" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C81" s="25">
         <v>372</v>
@@ -20259,7 +20256,7 @@
         <v>15</v>
       </c>
       <c r="E81" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F81" s="22" t="s">
         <v>117</v>
@@ -20298,29 +20295,29 @@
         <v>117</v>
       </c>
       <c r="R81" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="S81" s="10" t="s">
         <v>257</v>
-      </c>
-      <c r="S81" s="10" t="s">
-        <v>258</v>
       </c>
       <c r="T81" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U81" s="7"/>
       <c r="V81" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W81" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="X81" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y81" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z81" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA81" s="20" t="s">
         <v>3</v>
@@ -20468,7 +20465,7 @@
         <v>133</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C82" s="25">
         <v>500</v>
@@ -20480,7 +20477,7 @@
         <v>135</v>
       </c>
       <c r="F82" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G82" s="27">
         <v>1</v>
@@ -20489,19 +20486,19 @@
         <v>1</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="K82" s="13" t="s">
         <v>135</v>
       </c>
+      <c r="K82" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="L82" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="M82" s="13" t="s">
         <v>135</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="N82" s="14" t="s">
         <v>22</v>
@@ -20528,7 +20525,7 @@
         <v>43</v>
       </c>
       <c r="V82" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W82" s="20" t="s">
         <v>133</v>
@@ -20540,7 +20537,7 @@
         <v>2</v>
       </c>
       <c r="Z82" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AA82" s="20" t="s">
         <v>3</v>
@@ -20551,7 +20548,7 @@
         <v>134</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C83" s="25">
         <v>500</v>
@@ -20563,7 +20560,7 @@
         <v>135</v>
       </c>
       <c r="F83" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G83" s="27">
         <v>1</v>
@@ -20572,19 +20569,19 @@
         <v>1</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="K83" s="13" t="s">
         <v>135</v>
       </c>
+      <c r="K83" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="L83" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="M83" s="13" t="s">
         <v>135</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="N83" s="14" t="s">
         <v>22</v>
@@ -20611,7 +20608,7 @@
         <v>43</v>
       </c>
       <c r="V83" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W83" s="20" t="s">
         <v>134</v>
@@ -20623,7 +20620,7 @@
         <v>2</v>
       </c>
       <c r="Z83" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA83" s="20" t="s">
         <v>3</v>
@@ -20631,10 +20628,10 @@
     </row>
     <row r="84" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C84" s="25">
         <v>500</v>
@@ -20646,7 +20643,7 @@
         <v>135</v>
       </c>
       <c r="F84" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G84" s="27">
         <v>1</v>
@@ -20655,19 +20652,19 @@
         <v>1</v>
       </c>
       <c r="I84" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="K84" s="13" t="s">
         <v>135</v>
       </c>
+      <c r="K84" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="L84" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="M84" s="13" t="s">
         <v>135</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="N84" s="14" t="s">
         <v>22</v>
@@ -20694,19 +20691,19 @@
         <v>43</v>
       </c>
       <c r="V84" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W84" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="X84" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Y84" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z84" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA84" s="20" t="s">
         <v>3</v>
@@ -22540,10 +22537,10 @@
   <sheetData>
     <row r="1" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" s="25">
         <v>53</v>
@@ -22552,10 +22549,10 @@
         <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G1" s="27">
         <v>1</v>
@@ -22601,19 +22598,19 @@
       </c>
       <c r="U1" s="8"/>
       <c r="V1" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="W1" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="X1" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="Z1" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AA1" s="20" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Refactor dependo EPVs - tidy up, remove mac legacy formatting
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E7D1EB-9441-F242-8C30-7EE137F22435}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079BE36-6B4B-1C42-84C4-BE0CCA0ED471}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="1100" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="1060" windowWidth="35600" windowHeight="24760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="5" r:id="rId1"/>
@@ -504,9 +504,6 @@
     <t>Cavia</t>
   </si>
   <si>
-    <t>Macropus</t>
-  </si>
-  <si>
     <t>Craseonycteris</t>
   </si>
   <si>
@@ -882,12 +879,6 @@
     <t>dependo.176-heterohyrax</t>
   </si>
   <si>
-    <t>procavia</t>
-  </si>
-  <si>
-    <t>heterohyrax</t>
-  </si>
-  <si>
     <t>dependo.202-thamnophis</t>
   </si>
   <si>
@@ -913,6 +904,15 @@
   </si>
   <si>
     <t>dependo.36-phyllostomidae</t>
+  </si>
+  <si>
+    <t>Macropus eugenii</t>
+  </si>
+  <si>
+    <t>Procavia capensis</t>
+  </si>
+  <si>
+    <t>Heterohyrax</t>
   </si>
 </sst>
 </file>
@@ -3405,10 +3405,10 @@
   <dimension ref="A1:FH97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
+      <selection pane="bottomRight" activeCell="E53" sqref="A1:AA84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3447,28 +3447,28 @@
         <v>74</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>139</v>
@@ -3530,7 +3530,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="25">
         <v>0</v>
@@ -3539,10 +3539,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G2" s="27">
         <v>1</v>
@@ -3551,7 +3551,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>129</v>
@@ -3611,7 +3611,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="25">
         <v>1</v>
@@ -3623,7 +3623,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G3" s="25">
         <v>23</v>
@@ -3632,7 +3632,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>130</v>
@@ -3691,10 +3691,10 @@
     </row>
     <row r="4" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="25">
         <v>2</v>
@@ -3706,7 +3706,7 @@
         <v>127</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" s="25">
         <v>8</v>
@@ -3715,7 +3715,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>129</v>
@@ -3755,10 +3755,10 @@
         <v>32913662</v>
       </c>
       <c r="W4" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X4" s="20" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Y4" s="20" t="s">
         <v>2</v>
@@ -3775,7 +3775,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C5" s="25">
         <v>3</v>
@@ -3787,7 +3787,7 @@
         <v>16</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G5" s="25">
         <v>3</v>
@@ -3796,7 +3796,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>129</v>
@@ -3995,7 +3995,7 @@
         <v>111</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="25">
         <v>4</v>
@@ -4007,7 +4007,7 @@
         <v>109</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="27">
         <v>4</v>
@@ -4016,7 +4016,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>130</v>
@@ -4055,7 +4055,7 @@
         <v>27.9</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W6" s="20" t="s">
         <v>111</v>
@@ -4215,7 +4215,7 @@
         <v>110</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="25">
         <v>5</v>
@@ -4227,7 +4227,7 @@
         <v>109</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G7" s="27">
         <v>4</v>
@@ -4236,7 +4236,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>129</v>
@@ -4275,7 +4275,7 @@
         <v>27.9</v>
       </c>
       <c r="V7" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W7" s="20" t="s">
         <v>110</v>
@@ -4435,7 +4435,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="25">
         <v>6</v>
@@ -4444,10 +4444,10 @@
         <v>15</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G8" s="25">
         <v>1</v>
@@ -4456,7 +4456,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J8" s="13" t="s">
         <v>129</v>
@@ -4493,7 +4493,7 @@
       </c>
       <c r="U8" s="7"/>
       <c r="V8" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W8" s="20" t="s">
         <v>9</v>
@@ -4653,7 +4653,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C9" s="25">
         <v>7</v>
@@ -4665,7 +4665,7 @@
         <v>88</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G9" s="25">
         <v>1</v>
@@ -4674,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J9" s="13" t="s">
         <v>129</v>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="U9" s="7"/>
       <c r="V9" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W9" s="20" t="s">
         <v>10</v>
@@ -4871,7 +4871,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C10" s="25">
         <v>8</v>
@@ -4883,7 +4883,7 @@
         <v>89</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G10" s="25">
         <v>1</v>
@@ -4892,7 +4892,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J10" s="13" t="s">
         <v>129</v>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="U10" s="7"/>
       <c r="V10" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W10" s="20" t="s">
         <v>11</v>
@@ -5086,10 +5086,10 @@
     </row>
     <row r="11" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C11" s="25">
         <v>9</v>
@@ -5098,10 +5098,10 @@
         <v>83</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G11" s="25">
         <v>2</v>
@@ -5110,7 +5110,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>129</v>
@@ -5136,10 +5136,10 @@
       <c r="Q11" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S11" s="18" t="s">
+      <c r="R11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S11" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T11" s="8" t="s">
@@ -5147,13 +5147,13 @@
       </c>
       <c r="U11" s="7"/>
       <c r="V11" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W11" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="X11" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Y11" s="20" t="s">
         <v>2</v>
@@ -5307,7 +5307,7 @@
         <v>39</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" s="25">
         <v>10</v>
@@ -5319,7 +5319,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="27">
         <v>1</v>
@@ -5365,7 +5365,7 @@
       </c>
       <c r="U12" s="7"/>
       <c r="V12" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W12" s="20" t="s">
         <v>39</v>
@@ -5525,7 +5525,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C13" s="25">
         <v>11</v>
@@ -5537,7 +5537,7 @@
         <v>122</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G13" s="27">
         <v>3</v>
@@ -5572,10 +5572,10 @@
       <c r="Q13" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R13" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S13" s="18" t="s">
+      <c r="R13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T13" s="8" t="s">
@@ -5583,7 +5583,7 @@
       </c>
       <c r="U13" s="7"/>
       <c r="V13" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W13" s="20" t="s">
         <v>12</v>
@@ -5743,7 +5743,7 @@
         <v>65</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C14" s="25">
         <v>12</v>
@@ -5755,7 +5755,7 @@
         <v>86</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" s="25">
         <v>1</v>
@@ -5764,7 +5764,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J14" s="13" t="s">
         <v>129</v>
@@ -5790,10 +5790,10 @@
       <c r="Q14" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R14" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S14" s="18" t="s">
+      <c r="R14" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T14" s="8" t="s">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="U14" s="7"/>
       <c r="V14" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W14" s="20" t="s">
         <v>65</v>
@@ -5961,7 +5961,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C15" s="25">
         <v>13</v>
@@ -5973,7 +5973,7 @@
         <v>87</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G15" s="27">
         <v>3</v>
@@ -5982,7 +5982,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J15" s="13" t="s">
         <v>129</v>
@@ -6021,7 +6021,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V15" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W15" s="20" t="s">
         <v>8</v>
@@ -6181,7 +6181,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C16" s="25">
         <v>14</v>
@@ -6193,7 +6193,7 @@
         <v>87</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G16" s="27">
         <v>5</v>
@@ -6202,7 +6202,7 @@
         <v>5</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J16" s="13" t="s">
         <v>129</v>
@@ -6241,7 +6241,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W16" s="20" t="s">
         <v>27</v>
@@ -6401,7 +6401,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C17" s="25">
         <v>15</v>
@@ -6413,7 +6413,7 @@
         <v>106</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G17" s="27">
         <v>1</v>
@@ -6422,7 +6422,7 @@
         <v>1</v>
       </c>
       <c r="I17" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J17" s="13" t="s">
         <v>129</v>
@@ -6461,7 +6461,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W17" s="20" t="s">
         <v>80</v>
@@ -6621,7 +6621,7 @@
         <v>75</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C18" s="25">
         <v>16</v>
@@ -6633,7 +6633,7 @@
         <v>90</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G18" s="27">
         <v>5</v>
@@ -6642,7 +6642,7 @@
         <v>5</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>130</v>
@@ -6679,7 +6679,7 @@
       </c>
       <c r="U18" s="8"/>
       <c r="V18" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W18" s="20" t="s">
         <v>75</v>
@@ -6839,7 +6839,7 @@
         <v>126</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C19" s="25">
         <v>20</v>
@@ -6851,7 +6851,7 @@
         <v>82</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G19" s="27">
         <v>13</v>
@@ -6860,7 +6860,7 @@
         <v>13</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>131</v>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="U19" s="8"/>
       <c r="V19" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W19" s="20" t="s">
         <v>126</v>
@@ -7057,7 +7057,7 @@
         <v>81</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C20" s="25">
         <v>22</v>
@@ -7069,7 +7069,7 @@
         <v>82</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G20" s="27">
         <v>73</v>
@@ -7078,7 +7078,7 @@
         <v>76</v>
       </c>
       <c r="I20" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>131</v>
@@ -7117,7 +7117,7 @@
         <v>62</v>
       </c>
       <c r="V20" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W20" s="20" t="s">
         <v>81</v>
@@ -7274,10 +7274,10 @@
     </row>
     <row r="21" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C21" s="25">
         <v>23</v>
@@ -7289,7 +7289,7 @@
         <v>91</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G21" s="27">
         <v>5</v>
@@ -7298,7 +7298,7 @@
         <v>5</v>
       </c>
       <c r="I21" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>130</v>
@@ -7340,10 +7340,10 @@
         <v>26037535</v>
       </c>
       <c r="W21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="X21" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Y21" s="20" t="s">
         <v>2</v>
@@ -7494,22 +7494,22 @@
     </row>
     <row r="22" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="25">
         <v>26</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G22" s="27">
         <v>7</v>
@@ -7518,7 +7518,7 @@
         <v>11</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>130</v>
@@ -7560,10 +7560,10 @@
         <v>15085543</v>
       </c>
       <c r="W22" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="X22" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="Y22" s="20" t="s">
         <v>2</v>
@@ -7717,7 +7717,7 @@
         <v>64</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C23" s="25">
         <v>27</v>
@@ -7729,7 +7729,7 @@
         <v>92</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G23" s="27">
         <v>3</v>
@@ -7738,7 +7738,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J23" s="13" t="s">
         <v>129</v>
@@ -7764,10 +7764,10 @@
       <c r="Q23" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R23" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S23" s="18" t="s">
+      <c r="R23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S23" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T23" s="8" t="s">
@@ -7775,7 +7775,7 @@
       </c>
       <c r="U23" s="8"/>
       <c r="V23" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W23" s="20" t="s">
         <v>64</v>
@@ -7935,7 +7935,7 @@
         <v>78</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="25">
         <v>28</v>
@@ -7947,7 +7947,7 @@
         <v>93</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G24" s="27">
         <v>1</v>
@@ -7956,7 +7956,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>130</v>
@@ -7983,17 +7983,17 @@
         <v>117</v>
       </c>
       <c r="R24" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="S24" s="10" t="s">
         <v>222</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>223</v>
       </c>
       <c r="T24" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U24" s="8"/>
       <c r="V24" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W24" s="20" t="s">
         <v>78</v>
@@ -8150,10 +8150,10 @@
     </row>
     <row r="25" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C25" s="25">
         <v>36</v>
@@ -8165,7 +8165,7 @@
         <v>121</v>
       </c>
       <c r="F25" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G25" s="27">
         <v>1</v>
@@ -8201,23 +8201,23 @@
         <v>117</v>
       </c>
       <c r="R25" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>176</v>
-      </c>
-      <c r="S25" s="10" t="s">
-        <v>177</v>
       </c>
       <c r="T25" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U25" s="8"/>
       <c r="V25" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W25" s="20" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="X25" s="20" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="Y25" s="20" t="s">
         <v>2</v>
@@ -8368,10 +8368,10 @@
     </row>
     <row r="26" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C26" s="25">
         <v>37</v>
@@ -8383,7 +8383,7 @@
         <v>154</v>
       </c>
       <c r="F26" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G26" s="25">
         <v>1</v>
@@ -8392,7 +8392,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J26" s="13" t="s">
         <v>129</v>
@@ -8419,23 +8419,23 @@
         <v>117</v>
       </c>
       <c r="R26" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="S26" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>225</v>
       </c>
       <c r="T26" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U26" s="8"/>
       <c r="V26" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W26" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="X26" s="20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y26" s="20" t="s">
         <v>2</v>
@@ -8589,7 +8589,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C27" s="25">
         <v>40</v>
@@ -8601,7 +8601,7 @@
         <v>119</v>
       </c>
       <c r="F27" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G27" s="27">
         <v>1</v>
@@ -8610,7 +8610,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>130</v>
@@ -8637,11 +8637,11 @@
         <v>117</v>
       </c>
       <c r="R27" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="S27" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="S27" s="10" t="s">
-        <v>235</v>
-      </c>
       <c r="T27" s="8" t="s">
         <v>43</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>43</v>
       </c>
       <c r="V27" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W27" s="20" t="s">
         <v>120</v>
@@ -8809,7 +8809,7 @@
         <v>124</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C28" s="25">
         <v>42</v>
@@ -8821,7 +8821,7 @@
         <v>96</v>
       </c>
       <c r="F28" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G28" s="25">
         <v>1</v>
@@ -8830,7 +8830,7 @@
         <v>1</v>
       </c>
       <c r="I28" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J28" s="13" t="s">
         <v>129</v>
@@ -8856,10 +8856,10 @@
       <c r="Q28" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R28" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S28" s="18" t="s">
+      <c r="R28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S28" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T28" s="8" t="s">
@@ -8867,7 +8867,7 @@
       </c>
       <c r="U28" s="7"/>
       <c r="V28" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W28" s="20" t="s">
         <v>124</v>
@@ -9027,7 +9027,7 @@
         <v>123</v>
       </c>
       <c r="B29" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C29" s="25">
         <v>43</v>
@@ -9039,7 +9039,7 @@
         <v>125</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G29" s="25">
         <v>5</v>
@@ -9048,7 +9048,7 @@
         <v>5</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>129</v>
@@ -9074,10 +9074,10 @@
       <c r="Q29" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="R29" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="S29" s="18" t="s">
+      <c r="R29" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S29" s="11" t="s">
         <v>43</v>
       </c>
       <c r="T29" s="8" t="s">
@@ -9085,7 +9085,7 @@
       </c>
       <c r="U29" s="8"/>
       <c r="V29" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W29" s="20" t="s">
         <v>123</v>
@@ -9257,7 +9257,7 @@
         <v>104</v>
       </c>
       <c r="F30" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G30" s="27">
         <v>2</v>
@@ -9305,7 +9305,7 @@
         <v>34</v>
       </c>
       <c r="V30" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W30" s="20" t="s">
         <v>25</v>
@@ -9462,7 +9462,7 @@
     </row>
     <row r="31" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B31" s="25" t="s">
         <v>84</v>
@@ -9477,7 +9477,7 @@
         <v>104</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G31" s="27">
         <v>2</v>
@@ -9523,13 +9523,13 @@
       </c>
       <c r="U31" s="8"/>
       <c r="V31" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W31" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X31" s="20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y31" s="20" t="s">
         <v>2</v>
@@ -9680,10 +9680,10 @@
     </row>
     <row r="32" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C32" s="25">
         <v>46</v>
@@ -9695,7 +9695,7 @@
         <v>17</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G32" s="25">
         <v>1</v>
@@ -9704,7 +9704,7 @@
         <v>2</v>
       </c>
       <c r="I32" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>129</v>
@@ -9741,13 +9741,13 @@
       </c>
       <c r="U32" s="8"/>
       <c r="V32" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W32" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="X32" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Y32" s="20" t="s">
         <v>2</v>
@@ -9898,10 +9898,10 @@
     </row>
     <row r="33" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C33" s="25">
         <v>47</v>
@@ -9910,10 +9910,10 @@
         <v>15</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F33" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G33" s="27">
         <v>1</v>
@@ -9949,11 +9949,11 @@
         <v>117</v>
       </c>
       <c r="R33" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="S33" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="S33" s="10" t="s">
-        <v>246</v>
-      </c>
       <c r="T33" s="8" t="s">
         <v>43</v>
       </c>
@@ -9961,13 +9961,13 @@
         <v>43</v>
       </c>
       <c r="V33" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W33" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X33" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Y33" s="20" t="s">
         <v>2</v>
@@ -10118,10 +10118,10 @@
     </row>
     <row r="34" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C34" s="25">
         <v>48</v>
@@ -10133,7 +10133,7 @@
         <v>105</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G34" s="25" t="s">
         <v>117</v>
@@ -10179,13 +10179,13 @@
       </c>
       <c r="U34" s="8"/>
       <c r="V34" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W34" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X34" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Y34" s="20" t="s">
         <v>2</v>
@@ -10336,10 +10336,10 @@
     </row>
     <row r="35" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C35" s="25">
         <v>49</v>
@@ -10348,7 +10348,7 @@
         <v>15</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F35" s="22" t="s">
         <v>117</v>
@@ -10397,13 +10397,13 @@
       </c>
       <c r="U35" s="8"/>
       <c r="V35" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W35" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="X35" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Y35" s="20" t="s">
         <v>2</v>
@@ -10554,10 +10554,10 @@
     </row>
     <row r="36" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C36" s="25">
         <v>50</v>
@@ -10566,7 +10566,7 @@
         <v>21</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>117</v>
@@ -10605,23 +10605,23 @@
         <v>117</v>
       </c>
       <c r="R36" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T36" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U36" s="8"/>
       <c r="V36" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W36" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X36" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y36" s="20" t="s">
         <v>2</v>
@@ -10775,7 +10775,7 @@
         <v>128</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C37" s="25">
         <v>51</v>
@@ -10784,10 +10784,10 @@
         <v>21</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G37" s="25">
         <v>4</v>
@@ -10823,17 +10823,17 @@
         <v>117</v>
       </c>
       <c r="R37" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="S37" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="S37" s="10" t="s">
-        <v>183</v>
       </c>
       <c r="T37" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U37" s="8"/>
       <c r="V37" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W37" s="20" t="s">
         <v>128</v>
@@ -10990,10 +10990,10 @@
     </row>
     <row r="38" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C38" s="25">
         <v>54</v>
@@ -11005,7 +11005,7 @@
         <v>155</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G38" s="27">
         <v>3</v>
@@ -11051,13 +11051,13 @@
       </c>
       <c r="U38" s="8"/>
       <c r="V38" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W38" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="X38" s="20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y38" s="20" t="s">
         <v>2</v>
@@ -11208,10 +11208,10 @@
     </row>
     <row r="39" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" s="25">
         <v>55</v>
@@ -11223,7 +11223,7 @@
         <v>17</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G39" s="25" t="s">
         <v>117</v>
@@ -11269,13 +11269,13 @@
       </c>
       <c r="U39" s="8"/>
       <c r="V39" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W39" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="X39" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="Y39" s="20" t="s">
         <v>2</v>
@@ -11426,10 +11426,10 @@
     </row>
     <row r="40" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C40" s="25">
         <v>56</v>
@@ -11441,7 +11441,7 @@
         <v>107</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G40" s="27">
         <v>3</v>
@@ -11450,7 +11450,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J40" s="13" t="s">
         <v>129</v>
@@ -11486,13 +11486,13 @@
         <v>43</v>
       </c>
       <c r="V40" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W40" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="X40" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Y40" s="20" t="s">
         <v>2</v>
@@ -11643,10 +11643,10 @@
     </row>
     <row r="41" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C41" s="25">
         <v>58</v>
@@ -11655,7 +11655,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F41" s="22" t="s">
         <v>117</v>
@@ -11704,13 +11704,13 @@
       </c>
       <c r="U41" s="8"/>
       <c r="V41" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W41" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="X41" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Y41" s="20" t="s">
         <v>2</v>
@@ -11861,10 +11861,10 @@
     </row>
     <row r="42" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C42" s="25">
         <v>59</v>
@@ -11873,7 +11873,7 @@
         <v>83</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F42" s="22" t="s">
         <v>117</v>
@@ -11912,22 +11912,22 @@
         <v>117</v>
       </c>
       <c r="R42" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S42" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T42" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V42" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W42" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="X42" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="Y42" s="20" t="s">
         <v>2</v>
@@ -12078,10 +12078,10 @@
     </row>
     <row r="43" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C43" s="25">
         <v>60</v>
@@ -12090,10 +12090,10 @@
         <v>15</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G43" s="29">
         <v>1</v>
@@ -12141,13 +12141,13 @@
         <v>43</v>
       </c>
       <c r="V43" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W43" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X43" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Y43" s="20" t="s">
         <v>2</v>
@@ -12298,10 +12298,10 @@
     </row>
     <row r="44" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C44" s="25">
         <v>61</v>
@@ -12310,10 +12310,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G44" s="29">
         <v>1</v>
@@ -12361,13 +12361,13 @@
         <v>43</v>
       </c>
       <c r="V44" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W44" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X44" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Y44" s="20" t="s">
         <v>2</v>
@@ -12518,10 +12518,10 @@
     </row>
     <row r="45" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C45" s="25">
         <v>62</v>
@@ -12530,10 +12530,10 @@
         <v>15</v>
       </c>
       <c r="E45" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G45" s="29">
         <v>1</v>
@@ -12581,13 +12581,13 @@
         <v>43</v>
       </c>
       <c r="V45" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W45" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="X45" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Y45" s="20" t="s">
         <v>2</v>
@@ -12738,10 +12738,10 @@
     </row>
     <row r="46" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C46" s="25">
         <v>63</v>
@@ -12789,11 +12789,11 @@
         <v>116</v>
       </c>
       <c r="R46" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="S46" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="S46" s="10" t="s">
-        <v>194</v>
-      </c>
       <c r="T46" s="8" t="s">
         <v>43</v>
       </c>
@@ -12801,13 +12801,13 @@
         <v>43</v>
       </c>
       <c r="V46" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W46" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="X46" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="Y46" s="20" t="s">
         <v>2</v>
@@ -12958,10 +12958,10 @@
     </row>
     <row r="47" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C47" s="25">
         <v>64</v>
@@ -13019,13 +13019,13 @@
       </c>
       <c r="U47" s="8"/>
       <c r="V47" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W47" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="X47" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Y47" s="20" t="s">
         <v>2</v>
@@ -13176,10 +13176,10 @@
     </row>
     <row r="48" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C48" s="25">
         <v>75</v>
@@ -13188,7 +13188,7 @@
         <v>15</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F48" s="22" t="s">
         <v>117</v>
@@ -13237,13 +13237,13 @@
       </c>
       <c r="U48" s="8"/>
       <c r="V48" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W48" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="X48" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y48" s="20" t="s">
         <v>2</v>
@@ -13394,10 +13394,10 @@
     </row>
     <row r="49" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C49" s="25">
         <v>76</v>
@@ -13406,7 +13406,7 @@
         <v>21</v>
       </c>
       <c r="E49" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F49" s="22" t="s">
         <v>117</v>
@@ -13455,13 +13455,13 @@
       </c>
       <c r="U49" s="8"/>
       <c r="V49" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W49" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X49" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y49" s="20" t="s">
         <v>2</v>
@@ -13612,10 +13612,10 @@
     </row>
     <row r="50" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C50" s="25">
         <v>86</v>
@@ -13627,7 +13627,7 @@
         <v>119</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G50" s="25">
         <v>5</v>
@@ -13636,7 +13636,7 @@
         <v>5</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>130</v>
@@ -13663,11 +13663,11 @@
         <v>117</v>
       </c>
       <c r="R50" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="S50" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="S50" s="10" t="s">
-        <v>196</v>
-      </c>
       <c r="T50" s="8" t="s">
         <v>43</v>
       </c>
@@ -13675,13 +13675,13 @@
         <v>43</v>
       </c>
       <c r="V50" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W50" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X50" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Y50" s="20" t="s">
         <v>2</v>
@@ -13832,10 +13832,10 @@
     </row>
     <row r="51" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C51" s="25">
         <v>87</v>
@@ -13844,7 +13844,7 @@
         <v>15</v>
       </c>
       <c r="E51" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F51" s="22" t="s">
         <v>117</v>
@@ -13883,11 +13883,11 @@
         <v>117</v>
       </c>
       <c r="R51" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="S51" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="S51" s="10" t="s">
-        <v>239</v>
-      </c>
       <c r="T51" s="8" t="s">
         <v>43</v>
       </c>
@@ -13895,13 +13895,13 @@
         <v>43</v>
       </c>
       <c r="V51" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W51" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X51" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Y51" s="20" t="s">
         <v>2</v>
@@ -14052,10 +14052,10 @@
     </row>
     <row r="52" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C52" s="25">
         <v>88</v>
@@ -14064,7 +14064,7 @@
         <v>15</v>
       </c>
       <c r="E52" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F52" s="22" t="s">
         <v>117</v>
@@ -14099,25 +14099,25 @@
       <c r="P52" s="3"/>
       <c r="Q52" s="33"/>
       <c r="R52" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="S52" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="T52" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U52" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V52" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="W52" s="20" t="s">
         <v>272</v>
       </c>
-      <c r="S52" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="T52" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U52" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V52" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="W52" s="20" t="s">
-        <v>273</v>
-      </c>
       <c r="X52" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Y52" s="20" t="s">
         <v>2</v>
@@ -14268,10 +14268,10 @@
     </row>
     <row r="53" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C53" s="25">
         <v>92</v>
@@ -14280,10 +14280,10 @@
         <v>15</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G53" s="27">
         <v>1</v>
@@ -14316,13 +14316,13 @@
         <v>84</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R53" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S53" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T53" s="8" t="s">
         <v>43</v>
@@ -14331,13 +14331,13 @@
         <v>43</v>
       </c>
       <c r="V53" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W53" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="X53" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Y53" s="20" t="s">
         <v>2</v>
@@ -14488,10 +14488,10 @@
     </row>
     <row r="54" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C54" s="25">
         <v>100</v>
@@ -14500,7 +14500,7 @@
         <v>15</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F54" s="22" t="s">
         <v>117</v>
@@ -14539,23 +14539,23 @@
         <v>117</v>
       </c>
       <c r="R54" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S54" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="T54" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U54" s="8"/>
       <c r="V54" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W54" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="X54" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Y54" s="20" t="s">
         <v>2</v>
@@ -14706,10 +14706,10 @@
     </row>
     <row r="55" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C55" s="25">
         <v>160</v>
@@ -14721,7 +14721,7 @@
         <v>40</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G55" s="25">
         <v>1</v>
@@ -14730,7 +14730,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J55" s="13" t="s">
         <v>129</v>
@@ -14754,25 +14754,25 @@
         <v>84</v>
       </c>
       <c r="Q55" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="R55" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S55" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="T55" s="8" t="s">
         <v>43</v>
       </c>
       <c r="V55" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="W55" s="20" t="s">
         <v>213</v>
       </c>
-      <c r="W55" s="20" t="s">
-        <v>214</v>
-      </c>
       <c r="X55" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="Y55" s="20" t="s">
         <v>2</v>
@@ -14923,10 +14923,10 @@
     </row>
     <row r="56" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C56" s="25">
         <v>162</v>
@@ -14935,10 +14935,10 @@
         <v>15</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G56" s="27">
         <v>1</v>
@@ -14947,7 +14947,7 @@
         <v>1</v>
       </c>
       <c r="I56" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>129</v>
@@ -14987,10 +14987,10 @@
         <v>27377618</v>
       </c>
       <c r="W56" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="X56" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Y56" s="20" t="s">
         <v>2</v>
@@ -15141,10 +15141,10 @@
     </row>
     <row r="57" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C57" s="25">
         <v>163</v>
@@ -15153,10 +15153,10 @@
         <v>15</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G57" s="27">
         <v>1</v>
@@ -15165,7 +15165,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>129</v>
@@ -15205,10 +15205,10 @@
         <v>27377618</v>
       </c>
       <c r="W57" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="X57" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Y57" s="20" t="s">
         <v>2</v>
@@ -15359,10 +15359,10 @@
     </row>
     <row r="58" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C58" s="25">
         <v>164</v>
@@ -15371,10 +15371,10 @@
         <v>15</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="F58" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G58" s="27">
         <v>1</v>
@@ -15383,7 +15383,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>129</v>
@@ -15423,10 +15423,10 @@
         <v>27377618</v>
       </c>
       <c r="W58" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="X58" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Y58" s="20" t="s">
         <v>2</v>
@@ -15577,10 +15577,10 @@
     </row>
     <row r="59" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C59" s="25">
         <v>174</v>
@@ -15592,7 +15592,7 @@
         <v>153</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G59" s="27">
         <v>1</v>
@@ -15601,7 +15601,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J59" s="4" t="s">
         <v>43</v>
@@ -15628,11 +15628,11 @@
         <v>117</v>
       </c>
       <c r="R59" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="S59" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="S59" s="10" t="s">
-        <v>175</v>
-      </c>
       <c r="T59" s="8" t="s">
         <v>43</v>
       </c>
@@ -15640,13 +15640,13 @@
         <v>43</v>
       </c>
       <c r="V59" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W59" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X59" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Y59" s="20" t="s">
         <v>2</v>
@@ -15797,10 +15797,10 @@
     </row>
     <row r="60" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C60" s="25">
         <v>175</v>
@@ -15809,7 +15809,7 @@
         <v>15</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="F60" s="22" t="s">
         <v>117</v>
@@ -15858,13 +15858,13 @@
       </c>
       <c r="U60" s="8"/>
       <c r="V60" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W60" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="X60" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Y60" s="20" t="s">
         <v>2</v>
@@ -16015,10 +16015,10 @@
     </row>
     <row r="61" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C61" s="25">
         <v>176</v>
@@ -16027,7 +16027,7 @@
         <v>15</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="F61" s="22" t="s">
         <v>117</v>
@@ -16076,13 +16076,13 @@
       </c>
       <c r="U61" s="8"/>
       <c r="V61" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W61" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="X61" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Y61" s="20" t="s">
         <v>2</v>
@@ -16233,10 +16233,10 @@
     </row>
     <row r="62" spans="1:164" s="26" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C62" s="25">
         <v>180</v>
@@ -16245,10 +16245,10 @@
         <v>15</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G62" s="27">
         <v>2</v>
@@ -16257,7 +16257,7 @@
         <v>2</v>
       </c>
       <c r="I62" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>43</v>
@@ -16284,11 +16284,11 @@
         <v>117</v>
       </c>
       <c r="R62" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="S62" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="S62" s="10" t="s">
-        <v>185</v>
-      </c>
       <c r="T62" s="8" t="s">
         <v>43</v>
       </c>
@@ -16296,13 +16296,13 @@
         <v>43</v>
       </c>
       <c r="V62" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W62" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="X62" s="20" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Y62" s="20" t="s">
         <v>2</v>
@@ -16453,10 +16453,10 @@
     </row>
     <row r="63" spans="1:164" s="26" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C63" s="25">
         <v>187</v>
@@ -16465,10 +16465,10 @@
         <v>15</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G63" s="25">
         <v>1</v>
@@ -16504,11 +16504,11 @@
         <v>117</v>
       </c>
       <c r="R63" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="S63" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="S63" s="10" t="s">
-        <v>232</v>
-      </c>
       <c r="T63" s="8" t="s">
         <v>43</v>
       </c>
@@ -16516,13 +16516,13 @@
         <v>43</v>
       </c>
       <c r="V63" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W63" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="X63" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Y63" s="20" t="s">
         <v>2</v>
@@ -16673,10 +16673,10 @@
     </row>
     <row r="64" spans="1:164" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C64" s="25">
         <v>190</v>
@@ -16688,7 +16688,7 @@
         <v>40</v>
       </c>
       <c r="F64" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G64" s="25">
         <v>1</v>
@@ -16724,23 +16724,23 @@
         <v>117</v>
       </c>
       <c r="R64" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="S64" s="10" t="s">
         <v>241</v>
-      </c>
-      <c r="S64" s="10" t="s">
-        <v>242</v>
       </c>
       <c r="T64" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U64" s="7"/>
       <c r="V64" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W64" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X64" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y64" s="20" t="s">
         <v>2</v>
@@ -16891,10 +16891,10 @@
     </row>
     <row r="65" spans="1:164" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C65" s="25">
         <v>191</v>
@@ -16906,7 +16906,7 @@
         <v>40</v>
       </c>
       <c r="F65" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G65" s="25" t="s">
         <v>117</v>
@@ -16952,13 +16952,13 @@
       </c>
       <c r="U65" s="7"/>
       <c r="V65" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W65" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="X65" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Y65" s="20" t="s">
         <v>2</v>
@@ -17109,10 +17109,10 @@
     </row>
     <row r="66" spans="1:164" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C66" s="25">
         <v>192</v>
@@ -17124,7 +17124,7 @@
         <v>40</v>
       </c>
       <c r="F66" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G66" s="25" t="s">
         <v>117</v>
@@ -17169,13 +17169,13 @@
         <v>43</v>
       </c>
       <c r="V66" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W66" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="X66" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="Y66" s="20" t="s">
         <v>2</v>
@@ -17326,7 +17326,7 @@
     </row>
     <row r="67" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B67" s="25" t="s">
         <v>84</v>
@@ -17341,7 +17341,7 @@
         <v>94</v>
       </c>
       <c r="F67" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G67" s="29">
         <v>1</v>
@@ -17387,13 +17387,13 @@
       </c>
       <c r="U67" s="7"/>
       <c r="V67" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W67" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="X67" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Y67" s="20" t="s">
         <v>2</v>
@@ -17544,7 +17544,7 @@
     </row>
     <row r="68" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B68" s="25" t="s">
         <v>84</v>
@@ -17559,7 +17559,7 @@
         <v>94</v>
       </c>
       <c r="F68" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G68" s="29">
         <v>1</v>
@@ -17604,13 +17604,13 @@
         <v>43</v>
       </c>
       <c r="V68" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W68" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X68" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Y68" s="20" t="s">
         <v>2</v>
@@ -17761,7 +17761,7 @@
     </row>
     <row r="69" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B69" s="25" t="s">
         <v>84</v>
@@ -17776,7 +17776,7 @@
         <v>94</v>
       </c>
       <c r="F69" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G69" s="29">
         <v>1</v>
@@ -17822,13 +17822,13 @@
       </c>
       <c r="U69" s="7"/>
       <c r="V69" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W69" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="X69" s="20" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Y69" s="20" t="s">
         <v>2</v>
@@ -17979,10 +17979,10 @@
     </row>
     <row r="70" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C70" s="25">
         <v>201</v>
@@ -17994,7 +17994,7 @@
         <v>144</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G70" s="27">
         <v>1</v>
@@ -18003,7 +18003,7 @@
         <v>1</v>
       </c>
       <c r="I70" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>43</v>
@@ -18030,25 +18030,25 @@
         <v>117</v>
       </c>
       <c r="R70" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="S70" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="S70" s="10" t="s">
+      <c r="T70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="U70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="V70" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="W70" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="T70" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="U70" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V70" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="W70" s="20" t="s">
-        <v>180</v>
-      </c>
       <c r="X70" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Y70" s="20" t="s">
         <v>2</v>
@@ -18199,10 +18199,10 @@
     </row>
     <row r="71" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C71" s="25">
         <v>202</v>
@@ -18214,7 +18214,7 @@
         <v>144</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G71" s="27">
         <v>1</v>
@@ -18223,7 +18223,7 @@
         <v>1</v>
       </c>
       <c r="I71" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>43</v>
@@ -18250,11 +18250,11 @@
         <v>117</v>
       </c>
       <c r="R71" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="S71" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="S71" s="10" t="s">
-        <v>179</v>
-      </c>
       <c r="T71" s="8" t="s">
         <v>43</v>
       </c>
@@ -18262,13 +18262,13 @@
         <v>43</v>
       </c>
       <c r="V71" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W71" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="X71" s="20" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="Y71" s="20" t="s">
         <v>2</v>
@@ -18419,10 +18419,10 @@
     </row>
     <row r="72" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C72" s="25">
         <v>203</v>
@@ -18434,7 +18434,7 @@
         <v>145</v>
       </c>
       <c r="F72" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G72" s="27">
         <v>1</v>
@@ -18482,13 +18482,13 @@
         <v>43</v>
       </c>
       <c r="V72" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W72" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="X72" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Y72" s="20" t="s">
         <v>2</v>
@@ -18654,7 +18654,7 @@
         <v>151</v>
       </c>
       <c r="F73" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G73" s="27">
         <v>1</v>
@@ -18663,7 +18663,7 @@
         <v>1</v>
       </c>
       <c r="I73" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>43</v>
@@ -18690,10 +18690,10 @@
         <v>117</v>
       </c>
       <c r="R73" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="S73" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="T73" s="8" t="s">
         <v>43</v>
@@ -18702,7 +18702,7 @@
         <v>43</v>
       </c>
       <c r="V73" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W73" s="20" t="s">
         <v>150</v>
@@ -18859,10 +18859,10 @@
     </row>
     <row r="74" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C74" s="25">
         <v>365</v>
@@ -18874,7 +18874,7 @@
         <v>95</v>
       </c>
       <c r="F74" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G74" s="25">
         <v>7</v>
@@ -18883,7 +18883,7 @@
         <v>7</v>
       </c>
       <c r="I74" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>43</v>
@@ -18922,13 +18922,13 @@
         <v>43</v>
       </c>
       <c r="V74" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W74" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X74" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Y74" s="20" t="s">
         <v>2</v>
@@ -18942,10 +18942,10 @@
     </row>
     <row r="75" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C75" s="25">
         <v>366</v>
@@ -18957,7 +18957,7 @@
         <v>95</v>
       </c>
       <c r="F75" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G75" s="25">
         <v>20</v>
@@ -18966,7 +18966,7 @@
         <v>20</v>
       </c>
       <c r="I75" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>43</v>
@@ -19005,13 +19005,13 @@
         <v>43</v>
       </c>
       <c r="V75" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W75" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X75" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Y75" s="20" t="s">
         <v>2</v>
@@ -19162,10 +19162,10 @@
     </row>
     <row r="76" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C76" s="25">
         <v>367</v>
@@ -19174,10 +19174,10 @@
         <v>21</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F76" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G76" s="25" t="s">
         <v>117</v>
@@ -19221,13 +19221,13 @@
       </c>
       <c r="U76" s="7"/>
       <c r="V76" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W76" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="X76" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="Y76" s="20" t="s">
         <v>2</v>
@@ -19378,10 +19378,10 @@
     </row>
     <row r="77" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C77" s="25">
         <v>368</v>
@@ -19390,7 +19390,7 @@
         <v>21</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F77" s="22" t="s">
         <v>117</v>
@@ -19437,13 +19437,13 @@
       </c>
       <c r="U77" s="7"/>
       <c r="V77" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W77" s="20" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="X77" s="20" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Y77" s="20" t="s">
         <v>2</v>
@@ -19594,10 +19594,10 @@
     </row>
     <row r="78" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C78" s="25">
         <v>369</v>
@@ -19606,7 +19606,7 @@
         <v>15</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F78" s="22" t="s">
         <v>117</v>
@@ -19653,13 +19653,13 @@
       </c>
       <c r="U78" s="7"/>
       <c r="V78" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W78" s="20" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="X78" s="20" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="Y78" s="20" t="s">
         <v>2</v>
@@ -19810,10 +19810,10 @@
     </row>
     <row r="79" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C79" s="25">
         <v>370</v>
@@ -19825,7 +19825,7 @@
         <v>143</v>
       </c>
       <c r="F79" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G79" s="27">
         <v>1</v>
@@ -19834,7 +19834,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J79" s="13" t="s">
         <v>129</v>
@@ -19871,13 +19871,13 @@
       </c>
       <c r="U79" s="7"/>
       <c r="V79" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W79" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="X79" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Y79" s="20" t="s">
         <v>2</v>
@@ -20028,10 +20028,10 @@
     </row>
     <row r="80" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C80" s="25">
         <v>371</v>
@@ -20040,10 +20040,10 @@
         <v>15</v>
       </c>
       <c r="E80" s="23" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F80" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G80" s="25" t="s">
         <v>117</v>
@@ -20087,13 +20087,13 @@
       </c>
       <c r="U80" s="7"/>
       <c r="V80" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W80" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="X80" s="20" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="Y80" s="20" t="s">
         <v>2</v>
@@ -20244,10 +20244,10 @@
     </row>
     <row r="81" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B81" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C81" s="25">
         <v>372</v>
@@ -20256,7 +20256,7 @@
         <v>15</v>
       </c>
       <c r="E81" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F81" s="22" t="s">
         <v>117</v>
@@ -20295,23 +20295,23 @@
         <v>117</v>
       </c>
       <c r="R81" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="S81" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="S81" s="10" t="s">
-        <v>257</v>
       </c>
       <c r="T81" s="8" t="s">
         <v>43</v>
       </c>
       <c r="U81" s="7"/>
       <c r="V81" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W81" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="X81" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y81" s="20" t="s">
         <v>2</v>
@@ -20465,7 +20465,7 @@
         <v>133</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C82" s="25">
         <v>500</v>
@@ -20477,7 +20477,7 @@
         <v>135</v>
       </c>
       <c r="F82" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G82" s="27">
         <v>1</v>
@@ -20486,7 +20486,7 @@
         <v>1</v>
       </c>
       <c r="I82" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J82" s="13" t="s">
         <v>135</v>
@@ -20512,11 +20512,11 @@
       <c r="Q82" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R82" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S82" s="11" t="s">
-        <v>43</v>
+      <c r="R82" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="S82" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="T82" s="8" t="s">
         <v>43</v>
@@ -20525,7 +20525,7 @@
         <v>43</v>
       </c>
       <c r="V82" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W82" s="20" t="s">
         <v>133</v>
@@ -20548,7 +20548,7 @@
         <v>134</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C83" s="25">
         <v>500</v>
@@ -20560,7 +20560,7 @@
         <v>135</v>
       </c>
       <c r="F83" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G83" s="27">
         <v>1</v>
@@ -20569,7 +20569,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J83" s="13" t="s">
         <v>135</v>
@@ -20595,11 +20595,11 @@
       <c r="Q83" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R83" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S83" s="11" t="s">
-        <v>43</v>
+      <c r="R83" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="S83" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="T83" s="8" t="s">
         <v>43</v>
@@ -20608,7 +20608,7 @@
         <v>43</v>
       </c>
       <c r="V83" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W83" s="20" t="s">
         <v>134</v>
@@ -20631,7 +20631,7 @@
         <v>141</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C84" s="25">
         <v>500</v>
@@ -20643,7 +20643,7 @@
         <v>135</v>
       </c>
       <c r="F84" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G84" s="27">
         <v>1</v>
@@ -20652,7 +20652,7 @@
         <v>1</v>
       </c>
       <c r="I84" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J84" s="13" t="s">
         <v>135</v>
@@ -20678,11 +20678,11 @@
       <c r="Q84" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="R84" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="S84" s="11" t="s">
-        <v>43</v>
+      <c r="R84" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="S84" s="18" t="s">
+        <v>212</v>
       </c>
       <c r="T84" s="8" t="s">
         <v>43</v>
@@ -20691,7 +20691,7 @@
         <v>43</v>
       </c>
       <c r="V84" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W84" s="20" t="s">
         <v>141</v>
@@ -22537,10 +22537,10 @@
   <sheetData>
     <row r="1" spans="1:164" x14ac:dyDescent="0.2">
       <c r="A1" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="25">
         <v>53</v>
@@ -22549,10 +22549,10 @@
         <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G1" s="27">
         <v>1</v>
@@ -22598,13 +22598,13 @@
       </c>
       <c r="U1" s="8"/>
       <c r="V1" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="W1" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="X1" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Y1" s="20" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Fixed misspelling of Erythyro
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAF4E1B-4228-8D4A-B17A-83AC5A5E447B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322C1802-F684-EE42-859B-ADF4CC5B5A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="1360" windowWidth="28000" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="1340" windowWidth="28000" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="5" r:id="rId1"/>
@@ -3418,7 +3418,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="A1:AA77"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated phylogenies and web content
</commit_message>
<xml_diff>
--- a/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
+++ b/tabular/eve/parvovirinae/epv-dependo-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvovirus-GLUE/tabular/eve/parvovirinae/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7999D2AB-D686-5F4F-B27C-7BB6BFC75D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F008E25-1D10-074E-B594-DA1E4D73EE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3680" yWindow="1340" windowWidth="36660" windowHeight="26080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3419,10 +3419,10 @@
   <dimension ref="A1:FH92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:S13"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>